<commit_message>
Update folder names in MSLR Gauge Info spreadsheet
</commit_message>
<xml_diff>
--- a/M-S-and-L-Railway/MSLR_GaugeInfo.xlsx
+++ b/M-S-and-L-Railway/MSLR_GaugeInfo.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Git\BritishRainfall\M-S-and-L-Railway\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Git\Rainfall\MSLR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8215A9E-1D43-4C4A-A7A2-E95786865798}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0476293-F82C-40C9-9D4D-593197C6A717}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4447F5EC-047B-4B56-8205-9C000C53DF25}"/>
   </bookViews>
   <sheets>
-    <sheet name="Summary" sheetId="7" r:id="rId1"/>
+    <sheet name="Main Summary" sheetId="7" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Summary!$A$1:$R$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Main Summary'!$A$1:$R$55</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -89,6 +89,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="P48" authorId="0" shapeId="0" xr:uid="{2E46652D-5C7F-434E-803F-63FBEB3F1E96}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Richard:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+15/5 Now renamed STOCKWITH</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -318,9 +342,6 @@
     <t>GAINSBOROUGH-RAILWAY-STATION</t>
   </si>
   <si>
-    <t>GATE-BURTON-RAILWAY-STATION</t>
-  </si>
-  <si>
     <t>GRIMSBY-RAILWAY-STATION</t>
   </si>
   <si>
@@ -333,9 +354,6 @@
     <t>NEW-HOLLAND-RAILWAY-STATION</t>
   </si>
   <si>
-    <t>STOCKWITH-RAILWAY-STATION</t>
-  </si>
-  <si>
     <t>Starts</t>
   </si>
   <si>
@@ -408,6 +426,9 @@
     <t>Total</t>
   </si>
   <si>
+    <t>MSL&amp;R Gauge</t>
+  </si>
+  <si>
     <t>Is it a station ?</t>
   </si>
   <si>
@@ -447,7 +468,10 @@
     <t>Blank records for 1870-74 - nothing in British Rainfall either, so this gauge was out of action during this time.</t>
   </si>
   <si>
-    <t>MS&amp;LR Gauge</t>
+    <t>GATE-BURTON</t>
+  </si>
+  <si>
+    <t>STOCKWITH</t>
   </si>
 </sst>
 </file>
@@ -869,10 +893,10 @@
   <dimension ref="A1:R57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="P48" sqref="P48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,7 +916,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>23</v>
@@ -916,25 +940,25 @@
         <v>61</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="2"/>
       <c r="L1" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="O1" s="9"/>
       <c r="P1" s="3" t="s">
         <v>69</v>
       </c>
       <c r="Q1" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="R1" s="3" t="s">
         <v>68</v>
@@ -971,10 +995,10 @@
       <c r="J2" s="3"/>
       <c r="K2" s="2"/>
       <c r="L2" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N2" t="s">
         <v>4</v>
@@ -1014,10 +1038,10 @@
       <c r="J3" s="3"/>
       <c r="K3" s="2"/>
       <c r="L3" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N3" t="s">
         <v>4</v>
@@ -1057,10 +1081,10 @@
       <c r="J4" s="3"/>
       <c r="K4" s="2"/>
       <c r="L4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N4" s="5"/>
     </row>
@@ -1095,10 +1119,10 @@
       <c r="J5" s="3"/>
       <c r="K5" s="2"/>
       <c r="L5" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N5" t="s">
         <v>4</v>
@@ -1138,10 +1162,10 @@
       <c r="J6" s="3"/>
       <c r="K6" s="2"/>
       <c r="L6" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N6" t="s">
         <v>4</v>
@@ -1181,10 +1205,10 @@
       <c r="J7" s="3"/>
       <c r="K7" s="2"/>
       <c r="L7" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N7" t="s">
         <v>4</v>
@@ -1227,10 +1251,10 @@
       <c r="J8" s="3"/>
       <c r="K8" s="2"/>
       <c r="L8" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N8" t="s">
         <v>4</v>
@@ -1242,7 +1266,7 @@
         <v>4</v>
       </c>
       <c r="R8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1276,10 +1300,10 @@
       <c r="J9" s="3"/>
       <c r="K9" s="2"/>
       <c r="L9" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N9" t="s">
         <v>4</v>
@@ -1312,10 +1336,10 @@
       <c r="J10" s="3"/>
       <c r="K10" s="2"/>
       <c r="L10" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N10" s="5"/>
       <c r="Q10" t="s">
@@ -1353,10 +1377,10 @@
       <c r="J11" s="3"/>
       <c r="K11" s="2"/>
       <c r="L11" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N11" t="s">
         <v>4</v>
@@ -1364,7 +1388,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1394,7 +1418,7 @@
         <v>2</v>
       </c>
       <c r="R12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -1428,10 +1452,10 @@
       <c r="J13" s="3"/>
       <c r="K13" s="2"/>
       <c r="L13" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M13" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N13" t="s">
         <v>4</v>
@@ -1440,7 +1464,7 @@
         <v>2</v>
       </c>
       <c r="R13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -1472,10 +1496,10 @@
       <c r="J14" s="3"/>
       <c r="K14" s="2"/>
       <c r="L14" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M14" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N14" t="s">
         <v>4</v>
@@ -1484,7 +1508,7 @@
         <v>3</v>
       </c>
       <c r="R14" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -1518,10 +1542,10 @@
       <c r="J15" s="3"/>
       <c r="K15" s="2"/>
       <c r="L15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M15" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N15" s="5"/>
       <c r="Q15" t="s">
@@ -1559,10 +1583,10 @@
       <c r="J16" s="3"/>
       <c r="K16" s="2"/>
       <c r="L16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M16" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N16" s="5"/>
     </row>
@@ -1597,10 +1621,10 @@
       <c r="J17" s="3"/>
       <c r="K17" s="2"/>
       <c r="L17" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M17" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N17" t="s">
         <v>4</v>
@@ -1609,7 +1633,7 @@
         <v>4</v>
       </c>
       <c r="R17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -1643,10 +1667,10 @@
       <c r="J18" s="3"/>
       <c r="K18" s="2"/>
       <c r="L18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M18" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N18" s="5"/>
     </row>
@@ -1681,10 +1705,10 @@
       <c r="J19" s="3"/>
       <c r="K19" s="2"/>
       <c r="L19" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M19" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N19" t="s">
         <v>4</v>
@@ -1720,14 +1744,14 @@
       <c r="J20" s="3"/>
       <c r="K20" s="2"/>
       <c r="L20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="M20" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="N20" s="5"/>
       <c r="P20" t="s">
-        <v>74</v>
+        <v>116</v>
       </c>
       <c r="Q20" t="s">
         <v>2</v>
@@ -1764,16 +1788,16 @@
       <c r="J21" s="3"/>
       <c r="K21" s="2"/>
       <c r="L21" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M21" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N21" t="s">
         <v>4</v>
       </c>
       <c r="P21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -1801,10 +1825,10 @@
       <c r="J22" s="3"/>
       <c r="K22" s="2"/>
       <c r="L22" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="M22" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N22" s="5"/>
     </row>
@@ -1837,10 +1861,10 @@
       <c r="J23" s="3"/>
       <c r="K23" s="2"/>
       <c r="L23" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="M23" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N23" t="s">
         <v>4</v>
@@ -1849,7 +1873,7 @@
         <v>3</v>
       </c>
       <c r="R23" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
@@ -1883,16 +1907,16 @@
       <c r="J24" s="3"/>
       <c r="K24" s="2"/>
       <c r="L24" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M24" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N24" t="s">
         <v>4</v>
       </c>
       <c r="P24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q24" t="s">
         <v>4</v>
@@ -1925,10 +1949,10 @@
       <c r="J25" s="3"/>
       <c r="K25" s="2"/>
       <c r="L25" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M25" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N25" s="5"/>
       <c r="Q25" t="s">
@@ -1966,10 +1990,10 @@
       <c r="J26" s="3"/>
       <c r="K26" s="2"/>
       <c r="L26" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M26" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N26" t="s">
         <v>4</v>
@@ -2006,10 +2030,10 @@
       <c r="J27" s="3"/>
       <c r="K27" s="2"/>
       <c r="L27" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M27" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N27" t="s">
         <v>4</v>
@@ -2046,10 +2070,10 @@
       <c r="J28" s="3"/>
       <c r="K28" s="2"/>
       <c r="L28" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M28" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N28" t="s">
         <v>4</v>
@@ -2086,16 +2110,16 @@
       <c r="J29" s="3"/>
       <c r="K29" s="2"/>
       <c r="L29" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M29" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N29" t="s">
         <v>4</v>
       </c>
       <c r="P29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
@@ -2125,10 +2149,10 @@
       <c r="J30" s="3"/>
       <c r="K30" s="2"/>
       <c r="L30" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M30" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="N30" t="s">
         <v>4</v>
@@ -2168,10 +2192,10 @@
       <c r="J31" s="3"/>
       <c r="K31" s="2"/>
       <c r="L31" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M31" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N31" t="s">
         <v>4</v>
@@ -2210,10 +2234,10 @@
       <c r="J32" s="3"/>
       <c r="K32" s="2"/>
       <c r="L32" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M32" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="N32" s="5"/>
       <c r="Q32" t="s">
@@ -2251,10 +2275,10 @@
       <c r="J33" s="3"/>
       <c r="K33" s="2"/>
       <c r="L33" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M33" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N33" t="s">
         <v>4</v>
@@ -2263,7 +2287,7 @@
         <v>4</v>
       </c>
       <c r="R33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
@@ -2297,16 +2321,16 @@
       <c r="J34" s="3"/>
       <c r="K34" s="2"/>
       <c r="L34" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M34" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N34" t="s">
         <v>4</v>
       </c>
       <c r="P34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
@@ -2340,10 +2364,10 @@
       <c r="J35" s="3"/>
       <c r="K35" s="2"/>
       <c r="L35" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M35" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N35" t="s">
         <v>4</v>
@@ -2379,10 +2403,10 @@
       <c r="J36" s="3"/>
       <c r="K36" s="2"/>
       <c r="L36" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M36" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N36" s="5"/>
     </row>
@@ -2413,10 +2437,10 @@
       <c r="J37" s="3"/>
       <c r="K37" s="2"/>
       <c r="L37" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="M37" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N37" s="5"/>
       <c r="Q37" t="s">
@@ -2452,10 +2476,10 @@
       <c r="J38" s="3"/>
       <c r="K38" s="2"/>
       <c r="L38" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="M38" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N38" s="5"/>
       <c r="Q38" t="s">
@@ -2493,10 +2517,10 @@
       <c r="J39" s="3"/>
       <c r="K39" s="2"/>
       <c r="L39" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M39" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N39" t="s">
         <v>4</v>
@@ -2532,10 +2556,10 @@
       <c r="J40" s="3"/>
       <c r="K40" s="2"/>
       <c r="L40" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="M40" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="N40" s="5"/>
       <c r="P40" t="s">
@@ -2576,10 +2600,10 @@
       <c r="J41" s="3"/>
       <c r="K41" s="2"/>
       <c r="L41" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M41" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N41" t="s">
         <v>4</v>
@@ -2604,14 +2628,14 @@
       <c r="J42" s="3"/>
       <c r="K42" s="2"/>
       <c r="L42" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M42" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="N42" s="5"/>
       <c r="R42" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
@@ -2633,14 +2657,14 @@
       <c r="J43" s="3"/>
       <c r="K43" s="2"/>
       <c r="L43" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M43" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="N43" s="5"/>
       <c r="R43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
@@ -2670,17 +2694,17 @@
       <c r="J44" s="3"/>
       <c r="K44" s="2"/>
       <c r="L44" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M44" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="N44" s="5"/>
       <c r="Q44" t="s">
         <v>2</v>
       </c>
       <c r="R44" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
@@ -2712,17 +2736,17 @@
       <c r="J45" s="3"/>
       <c r="K45" s="2"/>
       <c r="L45" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="M45" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N45" s="5"/>
       <c r="Q45" t="s">
         <v>3</v>
       </c>
       <c r="R45" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
@@ -2756,10 +2780,10 @@
       <c r="J46" s="3"/>
       <c r="K46" s="2"/>
       <c r="L46" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M46" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N46" t="s">
         <v>4</v>
@@ -2768,7 +2792,7 @@
         <v>4</v>
       </c>
       <c r="R46" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
@@ -2798,10 +2822,10 @@
       <c r="J47" s="3"/>
       <c r="K47" s="2"/>
       <c r="L47" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M47" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N47" s="5"/>
       <c r="Q47" t="s">
@@ -2839,16 +2863,16 @@
       <c r="J48" s="3"/>
       <c r="K48" s="2"/>
       <c r="L48" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M48" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N48" t="s">
         <v>4</v>
       </c>
       <c r="P48" t="s">
-        <v>79</v>
+        <v>117</v>
       </c>
       <c r="Q48" t="s">
         <v>2</v>
@@ -2881,10 +2905,10 @@
       <c r="J49" s="3"/>
       <c r="K49" s="2"/>
       <c r="L49" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M49" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N49" s="5"/>
       <c r="Q49" t="s">
@@ -2922,10 +2946,10 @@
       <c r="J50" s="3"/>
       <c r="K50" s="2"/>
       <c r="L50" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M50" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N50" t="s">
         <v>4</v>
@@ -2965,10 +2989,10 @@
       <c r="J51" s="3"/>
       <c r="K51" s="2"/>
       <c r="L51" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M51" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N51" t="s">
         <v>4</v>
@@ -3011,16 +3035,16 @@
       <c r="J52" s="3"/>
       <c r="K52" s="2"/>
       <c r="L52" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M52" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N52" t="s">
         <v>4</v>
       </c>
       <c r="P52" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
@@ -3054,10 +3078,10 @@
       <c r="J53" s="3"/>
       <c r="K53" s="2"/>
       <c r="L53" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M53" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N53" s="5"/>
       <c r="Q53" t="s">
@@ -3091,10 +3115,10 @@
       <c r="J54" s="3"/>
       <c r="K54" s="2"/>
       <c r="L54" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="M54" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N54" s="5"/>
     </row>

</xml_diff>

<commit_message>
Add grid references for MS&LR locations to GaugeInfo spreadsheet
</commit_message>
<xml_diff>
--- a/M-S-and-L-Railway/MSLR_GaugeInfo.xlsx
+++ b/M-S-and-L-Railway/MSLR_GaugeInfo.xlsx
@@ -5,17 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Git\Rainfall\MSLR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Git\BritishRainfall\M-S-and-L-Railway\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0476293-F82C-40C9-9D4D-593197C6A717}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524E37CB-D818-482C-8B3B-4BB6C0ECE3DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4447F5EC-047B-4B56-8205-9C000C53DF25}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4447F5EC-047B-4B56-8205-9C000C53DF25}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Summary" sheetId="7" r:id="rId1"/>
+    <sheet name="Location Summary" sheetId="8" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Location Summary'!$A$1:$L$54</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Main Summary'!$A$1:$R$55</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -89,36 +91,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="P48" authorId="0" shapeId="0" xr:uid="{2E46652D-5C7F-434E-803F-63FBEB3F1E96}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Richard:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-15/5 Now renamed STOCKWITH</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="316">
   <si>
     <t>Lincoln</t>
   </si>
@@ -472,13 +450,607 @@
   </si>
   <si>
     <t>STOCKWITH</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Grouping</t>
+  </si>
+  <si>
+    <t>Altitude (ft)</t>
+  </si>
+  <si>
+    <t>Altitude (m)</t>
+  </si>
+  <si>
+    <t>Final Altitude (ft)</t>
+  </si>
+  <si>
+    <t>MS&amp;LR Network Type</t>
+  </si>
+  <si>
+    <t>Location Type</t>
+  </si>
+  <si>
+    <t>Gauge shown on map ?</t>
+  </si>
+  <si>
+    <t>Grid Reference</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Certainty</t>
+  </si>
+  <si>
+    <t>Map Links</t>
+  </si>
+  <si>
+    <t>Ashton Canal group</t>
+  </si>
+  <si>
+    <t>Canal network</t>
+  </si>
+  <si>
+    <t>Canal Lock</t>
+  </si>
+  <si>
+    <t>SD920010</t>
+  </si>
+  <si>
+    <t>Waterhouses had four locks</t>
+  </si>
+  <si>
+    <t>Rough location</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=18&amp;lat=53.50588&amp;lon=-2.12159&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>Lincolnshire Railway group</t>
+  </si>
+  <si>
+    <t>Railway network</t>
+  </si>
+  <si>
+    <t>Railway Station</t>
+  </si>
+  <si>
+    <t>TA053098</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.57522&amp;lon=-0.41022&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>South Yorkshire Waterways group</t>
+  </si>
+  <si>
+    <t>Canal Basin then Station</t>
+  </si>
+  <si>
+    <t>SE350070</t>
+  </si>
+  <si>
+    <t>Dearne and Dove Canal location initially, then moved to the Court House Station.</t>
+  </si>
+  <si>
+    <t>Best guess</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.55874&amp;lon=-1.47256&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>Peak Forest Canal group</t>
+  </si>
+  <si>
+    <t>Hill top</t>
+  </si>
+  <si>
+    <t>SJ970793</t>
+  </si>
+  <si>
+    <t>Rain Gauge marked on old OS Map near top of Sponds Hill.</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.31096&amp;lon=-2.04655&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>Macclesfield Canal group</t>
+  </si>
+  <si>
+    <t>SJ940662</t>
+  </si>
+  <si>
+    <t>Top of the hill' comment in 1848 report.</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.19330&amp;lon=-2.09051&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>Reservoir</t>
+  </si>
+  <si>
+    <t>SJ927657</t>
+  </si>
+  <si>
+    <t>Rain Gauge marked on old OS Map beside the reservoir at the eastern end.</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17.3&amp;lat=53.18856&amp;lon=-2.10940&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>TA004068</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.54929&amp;lon=-0.48558&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>Cable Railway Top</t>
+  </si>
+  <si>
+    <t>SK068803</t>
+  </si>
+  <si>
+    <t>Rain Gauge marked on old OS Map at the top of the Peak Forest Tramway's Inclined Plane.</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=18&amp;lat=53.31986&amp;lon=-1.89976&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>Cheshire Lines Railways group</t>
+  </si>
+  <si>
+    <t>SJ405670</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=18&amp;lat=53.19615&amp;lon=-2.89124&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>Chesterfield Canal group</t>
+  </si>
+  <si>
+    <t>Canal/Wharf then Station</t>
+  </si>
+  <si>
+    <t>SK387716</t>
+  </si>
+  <si>
+    <t>Canal location initially, then moved to the nearby railway station.</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.24038&amp;lon=-1.42144&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>Combs House</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Private House ?</t>
+  </si>
+  <si>
+    <t>SK043784</t>
+  </si>
+  <si>
+    <t>House not found on map. Only 10 months rainfall data, in 1855</t>
+  </si>
+  <si>
+    <t>Combs village guess</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.30298&amp;lon=-1.93642&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>SK059763</t>
+  </si>
+  <si>
+    <t>Rain Gauge marked on old OS Map near top of Combs Moss.</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.28409&amp;lon=-1.91222&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>SK035799</t>
+  </si>
+  <si>
+    <t>Rain Gauge marked on old OS Map near north-west corner of the reservoir.</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.31647&amp;lon=-1.94818&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>Canal Lock then Railway</t>
+  </si>
+  <si>
+    <t>SE835114</t>
+  </si>
+  <si>
+    <t>Stainforth and Keadby Canal Trent Lock initially, moved to railway land next door</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.59318&amp;lon=-0.74130&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>Canal then Railway</t>
+  </si>
+  <si>
+    <t>SE571036</t>
+  </si>
+  <si>
+    <t>Don Navigation New Cut location initially, then moved to railway property.</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=18&amp;lat=53.52612&amp;lon=-1.14044&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>Woodhead Railway group</t>
+  </si>
+  <si>
+    <t>SE158024</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.51758&amp;lon=-1.76333&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>SE387001</t>
+  </si>
+  <si>
+    <t>The Elsecar Branch of the Dearne and Dove Canal initially, then moved to a railway property</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=18&amp;lat=53.49631&amp;lon=-1.41723&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>SK819898</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.39956&amp;lon=-0.76993&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>Private residence group</t>
+  </si>
+  <si>
+    <t>Private residence</t>
+  </si>
+  <si>
+    <t>Private House</t>
+  </si>
+  <si>
+    <t>SK841833</t>
+  </si>
+  <si>
+    <t>George Morland Hutton, director of Great Central Railway, lived at Gate Burton</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.34037&amp;lon=-0.73761&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>TA268091</t>
+  </si>
+  <si>
+    <t>Grimsby Town Station</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.56367&amp;lon=-0.08679&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>Railway Bridge</t>
+  </si>
+  <si>
+    <t>SJ311695</t>
+  </si>
+  <si>
+    <t>Seems likely to refer to Hawarden Bridge over the Dee rather than the town, which is at far too high an altitude.</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.21750&amp;lon=-3.03250&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>SK472820</t>
+  </si>
+  <si>
+    <t>Norwood Locks where the Chesterfield Canal goes into a tunnel.</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.33352&amp;lon=-1.29263&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>SK973707</t>
+  </si>
+  <si>
+    <t>Lincoln St Mark's Station</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.22522&amp;lon=-0.54299&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>SJ343928</t>
+  </si>
+  <si>
+    <t>Became a goods station soon after opening.</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.42881&amp;lon=-2.99018&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>Canal side</t>
+  </si>
+  <si>
+    <t>SJ924727</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=18&amp;lat=53.25188&amp;lon=-2.11476&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>Canal Junction</t>
+  </si>
+  <si>
+    <t>SJ901979</t>
+  </si>
+  <si>
+    <t>Fairfield junction where the Ashton and Hollinwood canals meet.</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=18&amp;lat=53.47779&amp;lon=-2.14979&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>Canal Basin</t>
+  </si>
+  <si>
+    <t>SJ848981</t>
+  </si>
+  <si>
+    <t>A reference to the canal basin near Piccadilly (street) (by Dulcie Street at the junction with the Rochdale Canal) seems likely.</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=18&amp;lat=53.47971&amp;lon=-2.22958&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>TF107887</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.38440&amp;lon=-0.33806&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>Canal Aqueduct</t>
+  </si>
+  <si>
+    <t>SJ955900</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=18&amp;lat=53.40755&amp;lon=-2.06899&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>Canal Lock House</t>
+  </si>
+  <si>
+    <t>SJ962884</t>
+  </si>
+  <si>
+    <t>Lock House position is well defined.</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=18&amp;lat=53.39283&amp;lon=-2.05947&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>SJ989943</t>
+  </si>
+  <si>
+    <t>Hill End House, owned by MS&amp;LR's Chapman dynasty.Rain gauge shown on old OS map</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.44610&amp;lon=-2.01568&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>Field near Railway Station</t>
+  </si>
+  <si>
+    <t>SJ989937</t>
+  </si>
+  <si>
+    <t>Original rain gauge position marked on old OS Map at Matley's field near the station. Moved to Station in 1897</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=18&amp;lat=53.44067&amp;lon=-2.01577&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>TA081242</t>
+  </si>
+  <si>
+    <t>Rain Gauge marked on old OS Map at the old New Holland [Town] station.</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.70469&amp;lon=-0.36412&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>SJ956955</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=18&amp;lat=53.45685&amp;lon=-2.06718&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>SJ669739</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.26174&amp;lon=-2.49629&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>Railway Sidings</t>
+  </si>
+  <si>
+    <t>SD932037</t>
+  </si>
+  <si>
+    <t>No station. Railway and sidings near to the Lane's bridge over the tracks.</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.53026&amp;lon=-2.10362&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>Goods Shed</t>
+  </si>
+  <si>
+    <t>SE244034</t>
+  </si>
+  <si>
+    <t>Location near goods shed mentioned on final sheet.</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=18&amp;lat=53.52679&amp;lon=-1.63269&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>SE178033</t>
+  </si>
+  <si>
+    <t>John Chapman, Chairman and Director of MS&amp;LR, lived at Carlecotes Hall</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.52618&amp;lon=-1.73224&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>SE194028</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=18&amp;lat=53.52204&amp;lon=-1.70992&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>SK705808</t>
+  </si>
+  <si>
+    <t>Lock in the centre of  Retford</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=18&amp;lat=53.31909&amp;lon=-0.94283&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>Canal network ?</t>
+  </si>
+  <si>
+    <t>Canal Basin ?</t>
+  </si>
+  <si>
+    <t>SD899130</t>
+  </si>
+  <si>
+    <t>Only 2 years rainfall data, 1863-64</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.61390&amp;lon=-2.15339&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>SK426928</t>
+  </si>
+  <si>
+    <t>Rotherham Lock on Rotherham Cut</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=18&amp;lat=53.43074&amp;lon=-1.36062&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>SK340844</t>
+  </si>
+  <si>
+    <t>Seems to be a house called The Edge/Edge End. Owner unidentified</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.35555&amp;lon=-1.49078&amp;layers=6&amp;b=1</t>
+  </si>
+  <si>
+    <t>SK394901</t>
+  </si>
+  <si>
+    <t>Tinsley Locks Lock House, on the Sheffield and Tinsley Canal, initially, then moved to a railway location.</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.40626&amp;lon=-1.41062&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>SK361880</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=18&amp;lat=53.38769&amp;lon=-1.45865&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>SD331170</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.64571&amp;lon=-3.01232&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>SK785946</t>
+  </si>
+  <si>
+    <t>Basin where the canal meets the Trent</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.44300&amp;lon=-0.81993&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>SJ607886</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=18&amp;lat=53.39228&amp;lon=-2.59245&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>Reservoir dam</t>
+  </si>
+  <si>
+    <t>SK008812</t>
+  </si>
+  <si>
+    <t>Rain Gauge marked on old OS Map on the dam all at the eastern end of Toddbrook Reservoir</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=18&amp;lat=53.32784&amp;lon=-1.99017&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>SK112999</t>
+  </si>
+  <si>
+    <t>Rain Gauge marked on old OS Map next to the station.</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=18&amp;lat=53.49567&amp;lon=-1.83280&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>SK585792</t>
+  </si>
+  <si>
+    <t>Lock in the centre of Worksop. ['Station' added to sheets retrospectively, but not explained.]</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.30693&amp;lon=-1.12273&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>SE353034</t>
+  </si>
+  <si>
+    <t>Worsborough Basin at the end of the Worsborough Branch of the Dearne and Dove Canal</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.52664&amp;lon=-1.46830&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>SK299992</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=18&amp;lat=53.48849&amp;lon=-1.55083&amp;layers=168&amp;b=1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -520,6 +1092,42 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -559,10 +1167,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -576,11 +1185,1010 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="120">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -892,11 +2500,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CCABD69-03B3-436E-AEB0-0A7716EAF867}">
   <dimension ref="A1:R57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P48" sqref="P48"/>
+      <selection pane="bottomRight" activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3146,4 +4754,2201 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{550385DD-90D9-4324-8AF5-34DA66B6F837}">
+  <dimension ref="A1:L54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" style="22" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="22" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="116" style="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.28515625" style="22" customWidth="1"/>
+    <col min="12" max="12" width="29" style="22" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="22"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="21" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="22">
+        <v>345</v>
+      </c>
+      <c r="D2" s="22">
+        <v>105</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="H2" s="18"/>
+      <c r="I2" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="L2" s="23" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" s="22">
+        <v>51</v>
+      </c>
+      <c r="D3" s="22">
+        <v>16</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H3" s="18"/>
+      <c r="I3" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="L3" s="23" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="C4" s="22">
+        <v>175</v>
+      </c>
+      <c r="D4" s="22">
+        <v>53</v>
+      </c>
+      <c r="E4" s="22">
+        <v>317</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="H4" s="18"/>
+      <c r="I4" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="K4" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="L4" s="23" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" s="22">
+        <v>1279</v>
+      </c>
+      <c r="D5" s="22">
+        <v>390</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="K5" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="L5" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="C6" s="22">
+        <v>1210</v>
+      </c>
+      <c r="D6" s="22">
+        <v>369</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="H6" s="18"/>
+      <c r="I6" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="K6" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="L6" s="23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="C7" s="22">
+        <v>590</v>
+      </c>
+      <c r="D7" s="22">
+        <v>180</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="K7" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="L7" s="23" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8" s="22">
+        <v>16</v>
+      </c>
+      <c r="D8" s="22">
+        <v>5</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H8" s="18"/>
+      <c r="I8" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="L8" s="23" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="C9" s="22">
+        <v>965</v>
+      </c>
+      <c r="D9" s="22">
+        <v>294</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="J9" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="K9" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="L9" s="23" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="C10" s="22">
+        <v>84</v>
+      </c>
+      <c r="D10" s="22">
+        <v>26</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H10" s="18"/>
+      <c r="I10" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="23" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="C11" s="22">
+        <v>248</v>
+      </c>
+      <c r="D11" s="22">
+        <v>76</v>
+      </c>
+      <c r="E11" s="22">
+        <v>250</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="H11" s="18"/>
+      <c r="I11" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="K11" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="L11" s="24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="H12" s="18"/>
+      <c r="I12" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="J12" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="K12" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="L12" s="23" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="C13" s="22">
+        <v>1669</v>
+      </c>
+      <c r="D13" s="22">
+        <v>509</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="J13" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="K13" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="L13" s="23" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="C14" s="22">
+        <v>710</v>
+      </c>
+      <c r="D14" s="22">
+        <v>216</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="J14" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="K14" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="L14" s="23" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="C15" s="22">
+        <v>10</v>
+      </c>
+      <c r="D15" s="22">
+        <v>3</v>
+      </c>
+      <c r="E15" s="22">
+        <v>17</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="H15" s="18"/>
+      <c r="I15" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="J15" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="K15" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="L15" s="23" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="C16" s="22">
+        <v>35</v>
+      </c>
+      <c r="D16" s="22">
+        <v>11</v>
+      </c>
+      <c r="E16" s="22">
+        <v>32</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="H16" s="18"/>
+      <c r="I16" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="J16" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="K16" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="L16" s="23" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="C17" s="22">
+        <v>954</v>
+      </c>
+      <c r="D17" s="22">
+        <v>291</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H17" s="18"/>
+      <c r="I17" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="L17" s="23" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="C18" s="22">
+        <v>175</v>
+      </c>
+      <c r="D18" s="22">
+        <v>53</v>
+      </c>
+      <c r="E18" s="22">
+        <v>181</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="H18" s="18"/>
+      <c r="I18" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="J18" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="K18" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="L18" s="23" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="C19" s="22">
+        <v>76</v>
+      </c>
+      <c r="D19" s="22">
+        <v>23</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H19" s="18"/>
+      <c r="I19" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="L19" s="23" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="C20" s="22">
+        <v>96</v>
+      </c>
+      <c r="D20" s="22">
+        <v>29</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="H20" s="18"/>
+      <c r="I20" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="J20" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="K20" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="L20" s="23" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="C21" s="22">
+        <v>42</v>
+      </c>
+      <c r="D21" s="22">
+        <v>13</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H21" s="18"/>
+      <c r="I21" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="J21" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="K21" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="L21" s="23" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="C22" s="22">
+        <v>35</v>
+      </c>
+      <c r="D22" s="22">
+        <v>11</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="H22" s="18"/>
+      <c r="I22" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="J22" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="K22" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="L22" s="23" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="C23" s="22">
+        <v>238</v>
+      </c>
+      <c r="D23" s="22">
+        <v>73</v>
+      </c>
+      <c r="E23" s="22">
+        <v>226</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="H23" s="18"/>
+      <c r="I23" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="J23" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="K23" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="L23" s="23" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="C24" s="22">
+        <v>26</v>
+      </c>
+      <c r="D24" s="22">
+        <v>8</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H24" s="18"/>
+      <c r="I24" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="J24" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="K24" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="L24" s="23" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="C25" s="22">
+        <v>40</v>
+      </c>
+      <c r="D25" s="22">
+        <v>12</v>
+      </c>
+      <c r="E25" s="22">
+        <v>42</v>
+      </c>
+      <c r="F25" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="G25" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H25" s="18"/>
+      <c r="I25" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="J25" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="K25" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="L25" s="23" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="C26" s="22">
+        <v>539</v>
+      </c>
+      <c r="D26" s="22">
+        <v>164</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G26" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="H26" s="18"/>
+      <c r="I26" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="L26" s="23" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="C27" s="22">
+        <v>312</v>
+      </c>
+      <c r="D27" s="22">
+        <v>95</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="H27" s="18"/>
+      <c r="I27" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="J27" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="K27" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="L27" s="23" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="C28" s="22">
+        <v>194</v>
+      </c>
+      <c r="D28" s="22">
+        <v>59</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G28" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="H28" s="18"/>
+      <c r="I28" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="J28" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="K28" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="L28" s="23" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="C29" s="22">
+        <v>100</v>
+      </c>
+      <c r="D29" s="22">
+        <v>30</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="G29" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H29" s="18"/>
+      <c r="I29" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="L29" s="23" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="C30" s="22">
+        <v>321</v>
+      </c>
+      <c r="D30" s="22">
+        <v>98</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G30" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="H30" s="18"/>
+      <c r="I30" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="J30" s="17"/>
+      <c r="K30" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="L30" s="23" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="C31" s="22">
+        <v>543</v>
+      </c>
+      <c r="D31" s="22">
+        <v>166</v>
+      </c>
+      <c r="E31" s="22">
+        <v>523</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G31" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="J31" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="K31" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="L31" s="23" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="C32" s="22">
+        <v>600</v>
+      </c>
+      <c r="D32" s="22">
+        <v>183</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="G32" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="H32" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="I32" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="J32" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="K32" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="L32" s="23" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="C33" s="22">
+        <v>399</v>
+      </c>
+      <c r="D33" s="22">
+        <v>122</v>
+      </c>
+      <c r="E33" s="22">
+        <v>452</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="G33" s="17" t="s">
+        <v>251</v>
+      </c>
+      <c r="H33" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="I33" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="J33" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="K33" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="L33" s="23" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="C34" s="22">
+        <v>18</v>
+      </c>
+      <c r="D34" s="22">
+        <v>5</v>
+      </c>
+      <c r="F34" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="G34" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H34" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="I34" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="J34" s="17" t="s">
+        <v>256</v>
+      </c>
+      <c r="K34" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="L34" s="23" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="C35" s="25">
+        <v>396</v>
+      </c>
+      <c r="D35" s="22">
+        <v>121</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="G35" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H35" s="18"/>
+      <c r="I35" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="J35" s="17"/>
+      <c r="K35" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="L35" s="23" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="C36" s="22">
+        <v>76</v>
+      </c>
+      <c r="D36" s="22">
+        <v>23</v>
+      </c>
+      <c r="F36" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H36" s="18"/>
+      <c r="I36" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="J36" s="17"/>
+      <c r="K36" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="L36" s="23" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="C37" s="22">
+        <v>553</v>
+      </c>
+      <c r="D37" s="22">
+        <v>169</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="G37" s="17" t="s">
+        <v>262</v>
+      </c>
+      <c r="H37" s="18"/>
+      <c r="I37" s="17" t="s">
+        <v>263</v>
+      </c>
+      <c r="J37" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="K37" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="L37" s="24" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="C38" s="22">
+        <v>717</v>
+      </c>
+      <c r="D38" s="22">
+        <v>219</v>
+      </c>
+      <c r="F38" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="G38" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="H38" s="18"/>
+      <c r="I38" s="17" t="s">
+        <v>267</v>
+      </c>
+      <c r="J38" s="17" t="s">
+        <v>268</v>
+      </c>
+      <c r="K38" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="L38" s="23" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="C39" s="22">
+        <v>1075</v>
+      </c>
+      <c r="D39" s="22">
+        <v>328</v>
+      </c>
+      <c r="F39" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="G39" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="H39" s="18"/>
+      <c r="I39" s="17" t="s">
+        <v>270</v>
+      </c>
+      <c r="J39" s="17" t="s">
+        <v>271</v>
+      </c>
+      <c r="K39" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="L39" s="23" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="C40" s="22">
+        <v>868</v>
+      </c>
+      <c r="D40" s="22">
+        <v>265</v>
+      </c>
+      <c r="F40" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="G40" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H40" s="18"/>
+      <c r="I40" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="J40" s="17"/>
+      <c r="K40" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="L40" s="23" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="C41" s="25">
+        <v>52</v>
+      </c>
+      <c r="D41" s="22">
+        <v>16</v>
+      </c>
+      <c r="F41" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G41" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="H41" s="18"/>
+      <c r="I41" s="17" t="s">
+        <v>275</v>
+      </c>
+      <c r="J41" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="K41" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="L41" s="23" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B42" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="C42" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="D42" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="E42" s="25"/>
+      <c r="F42" s="17" t="s">
+        <v>278</v>
+      </c>
+      <c r="G42" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="H42" s="18"/>
+      <c r="I42" s="18" t="s">
+        <v>280</v>
+      </c>
+      <c r="J42" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="K42" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="L42" s="24" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B43" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="C43" s="22">
+        <v>85</v>
+      </c>
+      <c r="D43" s="22">
+        <v>26</v>
+      </c>
+      <c r="F43" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G43" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="H43" s="18"/>
+      <c r="I43" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="J43" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="K43" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="L43" s="23" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="C44" s="22">
+        <v>336</v>
+      </c>
+      <c r="D44" s="22">
+        <v>102</v>
+      </c>
+      <c r="F44" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="G44" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="H44" s="18"/>
+      <c r="I44" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="J44" s="17" t="s">
+        <v>287</v>
+      </c>
+      <c r="K44" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="L44" s="23" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="C45" s="22">
+        <v>143</v>
+      </c>
+      <c r="D45" s="22">
+        <v>44</v>
+      </c>
+      <c r="E45" s="22">
+        <v>117</v>
+      </c>
+      <c r="F45" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G45" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="H45" s="18"/>
+      <c r="I45" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="J45" s="17" t="s">
+        <v>290</v>
+      </c>
+      <c r="K45" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="L45" s="23" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="C46" s="25">
+        <v>188</v>
+      </c>
+      <c r="D46" s="22">
+        <v>6</v>
+      </c>
+      <c r="F46" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="G46" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H46" s="18"/>
+      <c r="I46" s="17" t="s">
+        <v>292</v>
+      </c>
+      <c r="J46" s="17"/>
+      <c r="K46" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="L46" s="23" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="C47" s="22">
+        <v>21</v>
+      </c>
+      <c r="D47" s="22">
+        <v>18</v>
+      </c>
+      <c r="F47" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="G47" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H47" s="18"/>
+      <c r="I47" s="17" t="s">
+        <v>294</v>
+      </c>
+      <c r="J47" s="17"/>
+      <c r="K47" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="L47" s="23" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="C48" s="25">
+        <v>21</v>
+      </c>
+      <c r="D48" s="22">
+        <v>6</v>
+      </c>
+      <c r="F48" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G48" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="H48" s="18"/>
+      <c r="I48" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="J48" s="17" t="s">
+        <v>297</v>
+      </c>
+      <c r="K48" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="L48" s="23" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="C49" s="22">
+        <v>59</v>
+      </c>
+      <c r="D49" s="22">
+        <v>18</v>
+      </c>
+      <c r="F49" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="G49" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H49" s="18"/>
+      <c r="I49" s="17" t="s">
+        <v>299</v>
+      </c>
+      <c r="J49" s="17"/>
+      <c r="K49" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="L49" s="23" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B50" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="C50" s="25">
+        <v>602</v>
+      </c>
+      <c r="D50" s="22">
+        <v>183</v>
+      </c>
+      <c r="F50" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G50" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="H50" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="I50" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="J50" s="17" t="s">
+        <v>303</v>
+      </c>
+      <c r="K50" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="L50" s="23" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="C51" s="22">
+        <v>939</v>
+      </c>
+      <c r="D51" s="22">
+        <v>286</v>
+      </c>
+      <c r="E51" s="22">
+        <v>878</v>
+      </c>
+      <c r="F51" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="G51" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H51" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="I51" s="17" t="s">
+        <v>305</v>
+      </c>
+      <c r="J51" s="17" t="s">
+        <v>306</v>
+      </c>
+      <c r="K51" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="L51" s="23" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B52" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="C52" s="25">
+        <v>127</v>
+      </c>
+      <c r="D52" s="22">
+        <v>39</v>
+      </c>
+      <c r="F52" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G52" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="H52" s="18"/>
+      <c r="I52" s="19" t="s">
+        <v>308</v>
+      </c>
+      <c r="J52" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="K52" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="L52" s="26" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B53" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="C53" s="22">
+        <v>225</v>
+      </c>
+      <c r="D53" s="22">
+        <v>69</v>
+      </c>
+      <c r="F53" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G53" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="H53" s="18"/>
+      <c r="I53" s="17" t="s">
+        <v>311</v>
+      </c>
+      <c r="J53" s="17" t="s">
+        <v>312</v>
+      </c>
+      <c r="K53" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="L53" s="23" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="C54" s="25">
+        <v>548</v>
+      </c>
+      <c r="D54" s="22">
+        <v>167</v>
+      </c>
+      <c r="F54" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="G54" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="I54" s="17" t="s">
+        <v>314</v>
+      </c>
+      <c r="J54" s="17"/>
+      <c r="K54" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="L54" s="23" t="s">
+        <v>315</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:L54" xr:uid="{F2A1E11B-C560-41D6-993C-5FE59B3DEE6A}"/>
+  <conditionalFormatting sqref="C54:E54">
+    <cfRule type="cellIs" dxfId="119" priority="1" operator="equal">
+      <formula>"Disagreement"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C52:E53 C47:E48 C41:E42 C37:E37 C33:E35 C29:E31 C23:E24 C21:E21 C19:E19 C16:E17 C11:E12 C6:E8 C3:E3 H1:I1 C1:E1">
+    <cfRule type="cellIs" dxfId="59" priority="59" operator="equal">
+      <formula>"Disagreement"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C52:E53 C47:E48 C41:E42 C37:E37 C33:E35 C29:E31 C23:E24 C21:E21 C19:E19 C16:E17 C11:E12 C6:E8 C3:E3 H1:I1 C1:E1">
+    <cfRule type="cellIs" dxfId="58" priority="60" operator="equal">
+      <formula>"ZZ999"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:E2">
+    <cfRule type="cellIs" dxfId="57" priority="57" operator="equal">
+      <formula>"Disagreement"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:E2">
+    <cfRule type="cellIs" dxfId="56" priority="58" operator="equal">
+      <formula>"ZZ999"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4:E4">
+    <cfRule type="cellIs" dxfId="55" priority="55" operator="equal">
+      <formula>"Disagreement"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4:E4">
+    <cfRule type="cellIs" dxfId="54" priority="56" operator="equal">
+      <formula>"ZZ999"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:E5">
+    <cfRule type="cellIs" dxfId="53" priority="53" operator="equal">
+      <formula>"Disagreement"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:E5">
+    <cfRule type="cellIs" dxfId="52" priority="54" operator="equal">
+      <formula>"ZZ999"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9:E9">
+    <cfRule type="cellIs" dxfId="51" priority="51" operator="equal">
+      <formula>"Disagreement"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9:E9">
+    <cfRule type="cellIs" dxfId="50" priority="52" operator="equal">
+      <formula>"ZZ999"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10:E10">
+    <cfRule type="cellIs" dxfId="49" priority="49" operator="equal">
+      <formula>"Disagreement"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10:E10">
+    <cfRule type="cellIs" dxfId="48" priority="50" operator="equal">
+      <formula>"ZZ999"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12:B12">
+    <cfRule type="cellIs" dxfId="47" priority="47" operator="equal">
+      <formula>"Disagreement"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12:B12">
+    <cfRule type="cellIs" dxfId="46" priority="48" operator="equal">
+      <formula>"ZZ999"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13:E13">
+    <cfRule type="cellIs" dxfId="45" priority="45" operator="equal">
+      <formula>"Disagreement"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13:E13">
+    <cfRule type="cellIs" dxfId="44" priority="46" operator="equal">
+      <formula>"ZZ999"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14:E14">
+    <cfRule type="cellIs" dxfId="43" priority="43" operator="equal">
+      <formula>"Disagreement"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14:E14">
+    <cfRule type="cellIs" dxfId="42" priority="44" operator="equal">
+      <formula>"ZZ999"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15:E15">
+    <cfRule type="cellIs" dxfId="41" priority="41" operator="equal">
+      <formula>"Disagreement"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15:E15">
+    <cfRule type="cellIs" dxfId="40" priority="42" operator="equal">
+      <formula>"ZZ999"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18:E18">
+    <cfRule type="cellIs" dxfId="39" priority="39" operator="equal">
+      <formula>"Disagreement"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18:E18">
+    <cfRule type="cellIs" dxfId="38" priority="40" operator="equal">
+      <formula>"ZZ999"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20:E20">
+    <cfRule type="cellIs" dxfId="37" priority="37" operator="equal">
+      <formula>"Disagreement"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20:E20">
+    <cfRule type="cellIs" dxfId="36" priority="38" operator="equal">
+      <formula>"ZZ999"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22:E22">
+    <cfRule type="cellIs" dxfId="35" priority="35" operator="equal">
+      <formula>"Disagreement"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22:E22">
+    <cfRule type="cellIs" dxfId="34" priority="36" operator="equal">
+      <formula>"ZZ999"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25:E25">
+    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
+      <formula>"Disagreement"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25:E25">
+    <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
+      <formula>"ZZ999"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C26:E26">
+    <cfRule type="cellIs" dxfId="31" priority="31" operator="equal">
+      <formula>"Disagreement"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C26:E26">
+    <cfRule type="cellIs" dxfId="30" priority="32" operator="equal">
+      <formula>"ZZ999"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27:E27">
+    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
+      <formula>"Disagreement"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27:E27">
+    <cfRule type="cellIs" dxfId="28" priority="30" operator="equal">
+      <formula>"ZZ999"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C28:E28">
+    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
+      <formula>"Disagreement"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C28:E28">
+    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
+      <formula>"ZZ999"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32:E32">
+    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
+      <formula>"Disagreement"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32:E32">
+    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
+      <formula>"ZZ999"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36:E36">
+    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
+      <formula>"Disagreement"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36:E36">
+    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
+      <formula>"ZZ999"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:E38">
+    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
+      <formula>"Disagreement"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:E38">
+    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
+      <formula>"ZZ999"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C39:E39">
+    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
+      <formula>"Disagreement"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C39:E39">
+    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
+      <formula>"ZZ999"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40:E40">
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+      <formula>"Disagreement"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40:E40">
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+      <formula>"ZZ999"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43:E43">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
+      <formula>"Disagreement"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43:E43">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+      <formula>"ZZ999"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C44:E44">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
+      <formula>"Disagreement"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C44:E44">
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+      <formula>"ZZ999"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C45:E45">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+      <formula>"Disagreement"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C45:E45">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+      <formula>"ZZ999"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C46:E46">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+      <formula>"Disagreement"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C46:E46">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>"ZZ999"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:E49">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>"Disagreement"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:E49">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+      <formula>"ZZ999"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50:E50">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"Disagreement"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50:E50">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"ZZ999"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51:E51">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"Disagreement"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51:E51">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"ZZ999"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54:E54">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"ZZ999"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1" location="zoom=18&amp;lat=53.50588&amp;lon=-2.12159&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.50588&amp;lon=-2.12159&amp;layers=168&amp;b=1" xr:uid="{9B894C87-2996-47E8-BFEB-A4158F3A85C5}"/>
+    <hyperlink ref="L3" r:id="rId2" location="zoom=17&amp;lat=53.57522&amp;lon=-0.41022&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.57522&amp;lon=-0.41022&amp;layers=168&amp;b=1" xr:uid="{3A932460-4663-40F0-BCCE-45984E9F098C}"/>
+    <hyperlink ref="L6" r:id="rId3" location="zoom=17&amp;lat=53.19330&amp;lon=-2.09051&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.19330&amp;lon=-2.09051&amp;layers=168&amp;b=1" xr:uid="{AE9BEDAE-1EB3-4A14-89F2-D512DAEB9FE0}"/>
+    <hyperlink ref="L7" r:id="rId4" location="zoom=17.3&amp;lat=53.18856&amp;lon=-2.10940&amp;layers=168&amp;b=1" xr:uid="{B44C0FDD-E0E1-40EA-9296-FDC8FD1E9D48}"/>
+    <hyperlink ref="L8" r:id="rId5" location="zoom=17&amp;lat=53.54929&amp;lon=-0.48558&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.54929&amp;lon=-0.48558&amp;layers=168&amp;b=1" xr:uid="{E1ED48FB-F1B2-4C9D-824B-10971F78FBB7}"/>
+    <hyperlink ref="L9" r:id="rId6" location="zoom=18&amp;lat=53.31986&amp;lon=-1.89976&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.31986&amp;lon=-1.89976&amp;layers=168&amp;b=1" xr:uid="{69573AD8-B3D0-46EF-A2A0-F5AAD631EF1E}"/>
+    <hyperlink ref="L10" r:id="rId7" location="zoom=18&amp;lat=53.19615&amp;lon=-2.89124&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.19615&amp;lon=-2.89124&amp;layers=168&amp;b=1" xr:uid="{EC1414AB-EA40-4A8E-859B-26AEE9D88C87}"/>
+    <hyperlink ref="L12" r:id="rId8" location="zoom=17&amp;lat=53.30298&amp;lon=-1.93642&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.30298&amp;lon=-1.93642&amp;layers=168&amp;b=1" xr:uid="{2A912195-2A8B-4051-B2A6-FC0BF7A51131}"/>
+    <hyperlink ref="L13" r:id="rId9" location="zoom=17&amp;lat=53.28409&amp;lon=-1.91222&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.28409&amp;lon=-1.91222&amp;layers=168&amp;b=1" xr:uid="{CCC042EE-2A34-4B58-8B5A-9906BCA88910}"/>
+    <hyperlink ref="L14" r:id="rId10" location="zoom=17&amp;lat=53.31647&amp;lon=-1.94818&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.31647&amp;lon=-1.94818&amp;layers=168&amp;b=1" xr:uid="{8BB2F39F-774C-4587-B7E0-61FFEDD3BD86}"/>
+    <hyperlink ref="L15" r:id="rId11" location="zoom=17&amp;lat=53.59318&amp;lon=-0.74130&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.59318&amp;lon=-0.74130&amp;layers=168&amp;b=1" xr:uid="{23BFDB11-7F7A-4197-960C-583EC17258E6}"/>
+    <hyperlink ref="L16" r:id="rId12" location="zoom=18&amp;lat=53.52612&amp;lon=-1.14044&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.52612&amp;lon=-1.14044&amp;layers=168&amp;b=1" xr:uid="{C416CD5F-BC4A-42E7-93C6-C94B65BFDF69}"/>
+    <hyperlink ref="L17" r:id="rId13" location="zoom=17&amp;lat=53.51758&amp;lon=-1.76333&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.51758&amp;lon=-1.76333&amp;layers=168&amp;b=1" xr:uid="{8EA5B3C4-FF54-4C32-A3DF-A30A81A254BA}"/>
+    <hyperlink ref="L18" r:id="rId14" location="zoom=18&amp;lat=53.49631&amp;lon=-1.41723&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.49631&amp;lon=-1.41723&amp;layers=168&amp;b=1" xr:uid="{E29FDE03-0E45-4938-955A-A08048B63E60}"/>
+    <hyperlink ref="L19" r:id="rId15" location="zoom=17&amp;lat=53.39956&amp;lon=-0.76993&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.39956&amp;lon=-0.76993&amp;layers=168&amp;b=1" xr:uid="{61ECAA8D-2931-4259-AD81-838456189860}"/>
+    <hyperlink ref="L20" r:id="rId16" location="zoom=17&amp;lat=53.34037&amp;lon=-0.73761&amp;layers=168&amp;b=1" display="zoom=17&amp;lat=53.34037&amp;lon=-0.73761&amp;layers=168&amp;b=1" xr:uid="{DB0067B6-CE6C-4EDC-B07C-D26E94C62F80}"/>
+    <hyperlink ref="L21" r:id="rId17" location="zoom=17&amp;lat=53.56367&amp;lon=-0.08679&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.56367&amp;lon=-0.08679&amp;layers=168&amp;b=1" xr:uid="{8B0420BE-BD8A-4321-BD82-B6F59BC35D5A}"/>
+    <hyperlink ref="L22" r:id="rId18" location="zoom=17&amp;lat=53.21750&amp;lon=-3.03250&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.21750&amp;lon=-3.03250&amp;layers=168&amp;b=1" xr:uid="{A5BA297F-B48F-41E7-A307-1D46476C6A36}"/>
+    <hyperlink ref="L23" r:id="rId19" location="zoom=17&amp;lat=53.33352&amp;lon=-1.29263&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.33352&amp;lon=-1.29263&amp;layers=168&amp;b=1" xr:uid="{943F15D6-2EDC-44DA-956C-C273B35A9FDC}"/>
+    <hyperlink ref="L24" r:id="rId20" location="zoom=17&amp;lat=53.22522&amp;lon=-0.54299&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.22522&amp;lon=-0.54299&amp;layers=168&amp;b=1" xr:uid="{C791D758-1DDF-4AA4-B40A-7FD8D6D74891}"/>
+    <hyperlink ref="L25" r:id="rId21" location="zoom=17&amp;lat=53.42881&amp;lon=-2.99018&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.42881&amp;lon=-2.99018&amp;layers=168&amp;b=1" xr:uid="{79BF8551-6673-4418-83FA-D4F7467E5671}"/>
+    <hyperlink ref="L26" r:id="rId22" location="zoom=18&amp;lat=53.25188&amp;lon=-2.11476&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.25188&amp;lon=-2.11476&amp;layers=168&amp;b=1" xr:uid="{7A36BB20-7096-4776-B194-41081EFD76F1}"/>
+    <hyperlink ref="L27" r:id="rId23" location="zoom=18&amp;lat=53.47779&amp;lon=-2.14979&amp;layers=168&amp;b=1" display="zoom=18&amp;lat=53.47779&amp;lon=-2.14979&amp;layers=168&amp;b=1" xr:uid="{1A68EFEB-3479-41E4-A6F1-45BBB485D43D}"/>
+    <hyperlink ref="L28" r:id="rId24" location="zoom=18&amp;lat=53.47971&amp;lon=-2.22958&amp;layers=168&amp;b=1" display="zoom=18&amp;lat=53.47971&amp;lon=-2.22958&amp;layers=168&amp;b=1" xr:uid="{7E0ACDA6-FAC8-4CDF-8FDD-5DB0B7C90DE1}"/>
+    <hyperlink ref="L29" r:id="rId25" location="zoom=17&amp;lat=53.38440&amp;lon=-0.33806&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.38440&amp;lon=-0.33806&amp;layers=168&amp;b=1" xr:uid="{95B84890-817E-4C65-9F82-C6376DD7E76C}"/>
+    <hyperlink ref="L30" r:id="rId26" location="zoom=18&amp;lat=53.40755&amp;lon=-2.06899&amp;layers=168&amp;b=1" xr:uid="{A9088DEA-9D72-4279-ACE6-4579AAC6255C}"/>
+    <hyperlink ref="L31" r:id="rId27" location="zoom=18&amp;lat=53.39283&amp;lon=-2.05947&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.39283&amp;lon=-2.05947&amp;layers=168&amp;b=1" xr:uid="{88357CC2-F767-41C5-9F18-47CFE5575D14}"/>
+    <hyperlink ref="L32" r:id="rId28" location="zoom=17&amp;lat=53.44610&amp;lon=-2.01568&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.44610&amp;lon=-2.01568&amp;layers=168&amp;b=1" xr:uid="{482E9D44-1BBC-4622-BF55-2280C82C4F69}"/>
+    <hyperlink ref="L33" r:id="rId29" location="zoom=18&amp;lat=53.44067&amp;lon=-2.01577&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.44067&amp;lon=-2.01577&amp;layers=168&amp;b=1" xr:uid="{E6603135-7879-4BA2-8FD7-469042B7E7E0}"/>
+    <hyperlink ref="L34" r:id="rId30" location="zoom=17&amp;lat=53.70469&amp;lon=-0.36412&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.70469&amp;lon=-0.36412&amp;layers=168&amp;b=1" xr:uid="{B807B8F4-E8EC-4E79-8C4B-4D5A93676033}"/>
+    <hyperlink ref="L35" r:id="rId31" location="zoom=18&amp;lat=53.45685&amp;lon=-2.06718&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.45685&amp;lon=-2.06718&amp;layers=168&amp;b=1" xr:uid="{A4F7F856-C870-4CA7-B810-81E0AC9BE366}"/>
+    <hyperlink ref="L36" r:id="rId32" location="zoom=17&amp;lat=53.26174&amp;lon=-2.49629&amp;layers=168&amp;b=1" display="zoom=17&amp;lat=53.26174&amp;lon=-2.49629&amp;layers=168&amp;b=1" xr:uid="{2D008E1F-4F05-4DC6-BA0E-90CA76AE9A33}"/>
+    <hyperlink ref="L38" r:id="rId33" location="zoom=18&amp;lat=53.52679&amp;lon=-1.63269&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.52679&amp;lon=-1.63269&amp;layers=168&amp;b=1" xr:uid="{5D178EE7-846E-4823-BEB5-5F0EFCFB1BD2}"/>
+    <hyperlink ref="L39" r:id="rId34" location="zoom=17&amp;lat=53.52618&amp;lon=-1.73224&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.52618&amp;lon=-1.73224&amp;layers=168&amp;b=1" xr:uid="{24F3EC29-7181-4A9B-9C5A-645FB433FFFE}"/>
+    <hyperlink ref="L40" r:id="rId35" location="zoom=18&amp;lat=53.52204&amp;lon=-1.70992&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.52204&amp;lon=-1.70992&amp;layers=168&amp;b=1" xr:uid="{27FB78A1-2CCA-4977-A322-BAD43ACE9E53}"/>
+    <hyperlink ref="L41" r:id="rId36" location="zoom=18&amp;lat=53.31880&amp;lon=-0.94143&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.31880&amp;lon=-0.94143&amp;layers=168&amp;b=1" xr:uid="{07123CEC-0031-42D2-ACE3-0A88DBC43A06}"/>
+    <hyperlink ref="L43" r:id="rId37" location="zoom=18&amp;lat=53.43074&amp;lon=-1.36062&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.43074&amp;lon=-1.36062&amp;layers=168&amp;b=1" xr:uid="{8A6AAC25-81AA-42AE-B8DD-0F632B56CE52}"/>
+    <hyperlink ref="L44" r:id="rId38" location="zoom=17&amp;lat=53.35555&amp;lon=-1.49078&amp;layers=6&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.35555&amp;lon=-1.49078&amp;layers=6&amp;b=1" xr:uid="{725A1FD7-B475-44EB-87AD-C93D5DE6151C}"/>
+    <hyperlink ref="L45" r:id="rId39" location="zoom=17&amp;lat=53.40626&amp;lon=-1.41062&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.40626&amp;lon=-1.41062&amp;layers=168&amp;b=1" xr:uid="{99F52E2A-9C75-42D9-B4C0-B1E8EB51E551}"/>
+    <hyperlink ref="L46" r:id="rId40" location="zoom=18&amp;lat=53.38769&amp;lon=-1.45865&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.38769&amp;lon=-1.45865&amp;layers=168&amp;b=1" xr:uid="{CEA44F0C-5B20-42C1-8DB8-D1CC7364EAA8}"/>
+    <hyperlink ref="L47" r:id="rId41" location="zoom=17&amp;lat=53.64571&amp;lon=-3.01232&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.64571&amp;lon=-3.01232&amp;layers=168&amp;b=1" xr:uid="{2B777C52-618D-42DC-A42C-51C45B3215FB}"/>
+    <hyperlink ref="L48" r:id="rId42" location="zoom=17&amp;lat=53.44300&amp;lon=-0.81993&amp;layers=168&amp;b=1" xr:uid="{96C4AD99-4E35-403D-A1CB-D53CE39CADBB}"/>
+    <hyperlink ref="L49" r:id="rId43" location="zoom=18&amp;lat=53.39228&amp;lon=-2.59245&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.39228&amp;lon=-2.59245&amp;layers=168&amp;b=1" xr:uid="{A385F51F-D7E6-44E8-B23A-08B45395411F}"/>
+    <hyperlink ref="L50" r:id="rId44" location="zoom=18&amp;lat=53.32784&amp;lon=-1.99017&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.32784&amp;lon=-1.99017&amp;layers=168&amp;b=1" xr:uid="{BBC7B1FD-E213-4B2D-9994-24234CDD4C28}"/>
+    <hyperlink ref="L51" r:id="rId45" location="zoom=18&amp;lat=53.49567&amp;lon=-1.83280&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.49567&amp;lon=-1.83280&amp;layers=168&amp;b=1" xr:uid="{8830D605-CD67-4E77-9DC3-A108B5D718FC}"/>
+    <hyperlink ref="L53" r:id="rId46" location="zoom=17&amp;lat=53.52664&amp;lon=-1.46830&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.52664&amp;lon=-1.46830&amp;layers=168&amp;b=1" xr:uid="{DA5F610B-1D5B-42E9-9721-0981C0544540}"/>
+    <hyperlink ref="L54" r:id="rId47" location="zoom=18&amp;lat=53.48849&amp;lon=-1.55083&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.48849&amp;lon=-1.55083&amp;layers=168&amp;b=1" xr:uid="{5B27AED8-71AA-46F6-8579-50F87BA43DE9}"/>
+    <hyperlink ref="L37" r:id="rId48" location="zoom=17&amp;lat=53.53026&amp;lon=-2.10362&amp;layers=168&amp;b=1" display="zoom=17&amp;lat=53.53026&amp;lon=-2.10362&amp;layers=168&amp;b=1" xr:uid="{5CE0239F-60FA-418E-8E2C-4F9A6FCB5B45}"/>
+    <hyperlink ref="L11" r:id="rId49" location="zoom=17&amp;lat=53.24038&amp;lon=-1.42144&amp;layers=168&amp;b=1" display="zoom=17&amp;lat=53.24038&amp;lon=-1.42144&amp;layers=168&amp;b=1" xr:uid="{4003A536-3F5A-450E-9AD8-9412E92B6060}"/>
+    <hyperlink ref="L52" r:id="rId50" location="zoom=17&amp;lat=53.30693&amp;lon=-1.12273&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.30693&amp;lon=-1.12273&amp;layers=168&amp;b=1" xr:uid="{C5CDAA38-1C18-48A6-AA11-FA85024A4DBB}"/>
+    <hyperlink ref="L42" r:id="rId51" location="zoom=17&amp;lat=53.61390&amp;lon=-2.15339&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.61390&amp;lon=-2.15339&amp;layers=168&amp;b=1" xr:uid="{F4068E9A-645F-424D-8BC0-7CC7F951F71F}"/>
+    <hyperlink ref="L5" r:id="rId52" location="zoom=17&amp;lat=53.31096&amp;lon=-2.04655&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.31096&amp;lon=-2.04655&amp;layers=168&amp;b=1" xr:uid="{F8D79F54-755B-4146-8981-12372D166779}"/>
+    <hyperlink ref="L4" r:id="rId53" location="zoom=17&amp;lat=53.55874&amp;lon=-1.47256&amp;layers=168&amp;b=1" xr:uid="{AFFAACBF-E426-4EFE-8807-1164163FA162}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update MSLR spreadsheet with further main GitHub cross-references
</commit_message>
<xml_diff>
--- a/M-S-and-L-Railway/MSLR_GaugeInfo.xlsx
+++ b/M-S-and-L-Railway/MSLR_GaugeInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Git\BritishRainfall\M-S-and-L-Railway\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A3677E-4396-4928-A2C1-2C09EB981FD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9488F9-002B-4DEF-BEA6-DDD27FE42AE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4447F5EC-047B-4B56-8205-9C000C53DF25}"/>
   </bookViews>
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="402">
   <si>
     <t>Lincoln</t>
   </si>
@@ -1292,6 +1292,42 @@
   </si>
   <si>
     <t>RR45</t>
+  </si>
+  <si>
+    <t>ASHTON-WATERHOUSES</t>
+  </si>
+  <si>
+    <t>DUNFORD-BRIDGE-STATION</t>
+  </si>
+  <si>
+    <t>KILLAMARSH-NORWOOD</t>
+  </si>
+  <si>
+    <t>MACCLESFIELD</t>
+  </si>
+  <si>
+    <t>MANCHESTER-FAIRFIELD</t>
+  </si>
+  <si>
+    <t>SHEFFIELD-VICTORIA</t>
+  </si>
+  <si>
+    <t>WHALEY-BRIDGE</t>
+  </si>
+  <si>
+    <t>RR144</t>
+  </si>
+  <si>
+    <t>RR142</t>
+  </si>
+  <si>
+    <t>RR145</t>
+  </si>
+  <si>
+    <t>RR146</t>
+  </si>
+  <si>
+    <t>RR141</t>
   </si>
 </sst>
 </file>
@@ -1735,15 +1771,9 @@
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2562,7 +2592,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R8" sqref="R8"/>
+      <selection pane="bottomRight" activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2684,6 +2714,12 @@
       <c r="P2" t="s">
         <v>2</v>
       </c>
+      <c r="Q2" t="s">
+        <v>390</v>
+      </c>
+      <c r="R2" s="115" t="s">
+        <v>401</v>
+      </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -3414,6 +3450,9 @@
       <c r="P17" t="s">
         <v>3</v>
       </c>
+      <c r="Q17" t="s">
+        <v>391</v>
+      </c>
       <c r="S17" t="s">
         <v>93</v>
       </c>
@@ -3705,6 +3744,12 @@
       <c r="P23" t="s">
         <v>2</v>
       </c>
+      <c r="Q23" t="s">
+        <v>392</v>
+      </c>
+      <c r="R23" s="115" t="s">
+        <v>400</v>
+      </c>
       <c r="S23" s="6" t="s">
         <v>94</v>
       </c>
@@ -3846,6 +3891,12 @@
       <c r="P26" t="s">
         <v>2</v>
       </c>
+      <c r="Q26" t="s">
+        <v>393</v>
+      </c>
+      <c r="R26" s="115" t="s">
+        <v>399</v>
+      </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
@@ -3893,6 +3944,12 @@
       </c>
       <c r="P27" t="s">
         <v>2</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>394</v>
+      </c>
+      <c r="R27" s="115" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
@@ -4769,6 +4826,12 @@
       <c r="P46" t="s">
         <v>3</v>
       </c>
+      <c r="Q46" t="s">
+        <v>395</v>
+      </c>
+      <c r="R46" s="115" t="s">
+        <v>397</v>
+      </c>
       <c r="S46" t="s">
         <v>100</v>
       </c>
@@ -4951,6 +5014,12 @@
       </c>
       <c r="P50" t="s">
         <v>2</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>396</v>
+      </c>
+      <c r="R50" s="115">
+        <v>2731</v>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Additional MS&LR sheets from 1840s. Just keep the combined sheet, remove the date-split ones.
</commit_message>
<xml_diff>
--- a/M-S-and-L-Railway/MSLR_GaugeInfo.xlsx
+++ b/M-S-and-L-Railway/MSLR_GaugeInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Git\BritishRainfall\M-S-and-L-Railway\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5632A863-CCBA-4D45-8ECE-0C60E19AC2CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF03B7D-22F3-41CB-9A32-DC5D6554D2D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4447F5EC-047B-4B56-8205-9C000C53DF25}"/>
   </bookViews>
@@ -1234,9 +1234,6 @@
     <t>RR89</t>
   </si>
   <si>
-    <t>RR89/RR90</t>
-  </si>
-  <si>
     <t>RR90</t>
   </si>
   <si>
@@ -1367,6 +1364,9 @@
   </si>
   <si>
     <t>The Aqueduct itself</t>
+  </si>
+  <si>
+    <t>2643/6/3/1</t>
   </si>
 </sst>
 </file>
@@ -2634,10 +2634,10 @@
   <dimension ref="A1:S57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q52" sqref="Q52"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2760,10 +2760,10 @@
         <v>2</v>
       </c>
       <c r="Q2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="R2" s="115" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -2862,7 +2862,7 @@
         <v>2</v>
       </c>
       <c r="Q4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -3129,7 +3129,7 @@
         <v>321</v>
       </c>
       <c r="R9" s="116" t="s">
-        <v>370</v>
+        <v>414</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -3218,7 +3218,7 @@
         <v>2</v>
       </c>
       <c r="Q11" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -3362,7 +3362,7 @@
         <v>323</v>
       </c>
       <c r="R14" s="116" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="S14" s="6" t="s">
         <v>92</v>
@@ -3412,10 +3412,10 @@
         <v>2</v>
       </c>
       <c r="Q15" t="s">
+        <v>405</v>
+      </c>
+      <c r="R15" s="115" t="s">
         <v>406</v>
-      </c>
-      <c r="R15" s="115" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -3462,10 +3462,10 @@
         <v>2</v>
       </c>
       <c r="Q16" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="R16" s="115" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
@@ -3514,10 +3514,10 @@
         <v>3</v>
       </c>
       <c r="Q17" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="R17" s="115" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="S17" t="s">
         <v>93</v>
@@ -3570,7 +3570,7 @@
         <v>324</v>
       </c>
       <c r="R18" s="115" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
@@ -3622,7 +3622,7 @@
         <v>64</v>
       </c>
       <c r="R19" s="116" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
@@ -3668,7 +3668,7 @@
         <v>101</v>
       </c>
       <c r="R20" s="116" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
@@ -3720,7 +3720,7 @@
         <v>65</v>
       </c>
       <c r="R21" s="116" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
@@ -3764,7 +3764,7 @@
         <v>325</v>
       </c>
       <c r="R22" s="116" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
@@ -3811,10 +3811,10 @@
         <v>2</v>
       </c>
       <c r="Q23" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="R23" s="115" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="S23" s="6" t="s">
         <v>94</v>
@@ -3869,7 +3869,7 @@
         <v>66</v>
       </c>
       <c r="R24" s="116" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
@@ -3958,10 +3958,10 @@
         <v>2</v>
       </c>
       <c r="Q26" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="R26" s="115" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
@@ -4012,10 +4012,10 @@
         <v>2</v>
       </c>
       <c r="Q27" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="R27" s="115" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
@@ -4067,7 +4067,7 @@
         <v>326</v>
       </c>
       <c r="R28" s="116" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
@@ -4119,7 +4119,7 @@
         <v>67</v>
       </c>
       <c r="R29" s="116" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
@@ -4167,7 +4167,7 @@
         <v>359</v>
       </c>
       <c r="R30" s="115" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
@@ -4221,7 +4221,7 @@
         <v>57</v>
       </c>
       <c r="R31" s="116" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
@@ -4313,7 +4313,7 @@
         <v>360</v>
       </c>
       <c r="R33" s="115" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="S33" t="s">
         <v>95</v>
@@ -4368,7 +4368,7 @@
         <v>68</v>
       </c>
       <c r="R34" s="116" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
@@ -4420,7 +4420,7 @@
         <v>38</v>
       </c>
       <c r="R35" s="116" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
@@ -4552,7 +4552,7 @@
         <v>61</v>
       </c>
       <c r="R38" s="116" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
@@ -4598,7 +4598,7 @@
         <v>58</v>
       </c>
       <c r="R39" s="116" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
@@ -4689,10 +4689,10 @@
         <v>2</v>
       </c>
       <c r="Q41" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="R41" s="115" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
@@ -4899,10 +4899,10 @@
         <v>3</v>
       </c>
       <c r="Q46" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="R46" s="115" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="S46" t="s">
         <v>100</v>
@@ -4997,7 +4997,7 @@
         <v>102</v>
       </c>
       <c r="R48" s="116" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
@@ -5088,7 +5088,7 @@
         <v>2</v>
       </c>
       <c r="Q50" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="R50" s="115">
         <v>2731</v>
@@ -5145,7 +5145,7 @@
         <v>59</v>
       </c>
       <c r="R51" s="116" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
@@ -5197,7 +5197,7 @@
         <v>87</v>
       </c>
       <c r="R52" s="116" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
@@ -5244,10 +5244,10 @@
         <v>2</v>
       </c>
       <c r="Q53" t="s">
+        <v>409</v>
+      </c>
+      <c r="R53" s="116" t="s">
         <v>410</v>
-      </c>
-      <c r="R53" s="116" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
@@ -5326,14 +5326,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{550385DD-90D9-4324-8AF5-34DA66B6F837}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:L54"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomRight" activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5424,7 +5423,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>7</v>
       </c>
@@ -5594,7 +5593,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>5</v>
       </c>
@@ -5660,7 +5659,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>43</v>
       </c>
@@ -5725,7 +5724,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>161</v>
       </c>
@@ -5900,7 +5899,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -5967,7 +5966,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="26" t="s">
         <v>23</v>
       </c>
@@ -5998,7 +5997,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="26" t="s">
         <v>22</v>
       </c>
@@ -6031,7 +6030,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
         <v>6</v>
       </c>
@@ -6064,7 +6063,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
         <v>53</v>
       </c>
@@ -6133,7 +6132,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
         <v>0</v>
       </c>
@@ -6166,7 +6165,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>45</v>
       </c>
@@ -6226,7 +6225,7 @@
         <v>214</v>
       </c>
       <c r="J26" s="16" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K26" s="16" t="s">
         <v>132</v>
@@ -6301,7 +6300,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="26" t="s">
         <v>4</v>
       </c>
@@ -6356,7 +6355,7 @@
         <v>227</v>
       </c>
       <c r="J30" s="16" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="K30" s="16" t="s">
         <v>126</v>
@@ -6401,7 +6400,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="26" t="s">
         <v>28</v>
       </c>
@@ -6436,7 +6435,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="26" t="s">
         <v>27</v>
       </c>
@@ -6474,7 +6473,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="26" t="s">
         <v>8</v>
       </c>
@@ -6509,7 +6508,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="26" t="s">
         <v>15</v>
       </c>
@@ -6540,7 +6539,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="26" t="s">
         <v>42</v>
       </c>
@@ -6571,7 +6570,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>47</v>
       </c>
@@ -6604,7 +6603,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="26" t="s">
         <v>19</v>
       </c>
@@ -6637,7 +6636,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>48</v>
       </c>
@@ -6670,7 +6669,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="26" t="s">
         <v>55</v>
       </c>
@@ -6801,7 +6800,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>51</v>
       </c>
@@ -6870,7 +6869,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="28" t="s">
         <v>52</v>
       </c>
@@ -6901,7 +6900,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="26" t="s">
         <v>50</v>
       </c>
@@ -6965,7 +6964,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>44</v>
       </c>
@@ -7031,7 +7030,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>21</v>
       </c>
@@ -7135,7 +7134,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>49</v>
       </c>
@@ -7166,14 +7165,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L54" xr:uid="{F2A1E11B-C560-41D6-993C-5FE59B3DEE6A}">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="Canal network"/>
-        <filter val="Canal network ?"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:L54" xr:uid="{F2A1E11B-C560-41D6-993C-5FE59B3DEE6A}"/>
   <conditionalFormatting sqref="C54:E54">
     <cfRule type="cellIs" dxfId="59" priority="1" operator="equal">
       <formula>"Disagreement"</formula>

</xml_diff>

<commit_message>
A few updates to MS&LR information
</commit_message>
<xml_diff>
--- a/M-S-and-L-Railway/MSLR_GaugeInfo.xlsx
+++ b/M-S-and-L-Railway/MSLR_GaugeInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Git\BritishRainfall\M-S-and-L-Railway\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58995F32-1E48-44B4-AE47-B32DB7EEC271}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE8C558-0BF4-4D1A-AD7C-2BF040421CE9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4447F5EC-047B-4B56-8205-9C000C53DF25}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{4447F5EC-047B-4B56-8205-9C000C53DF25}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Summary" sheetId="7" r:id="rId1"/>
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="440">
   <si>
     <t>Lincoln</t>
   </si>
@@ -513,18 +513,9 @@
     <t>Canal Basin then Station</t>
   </si>
   <si>
-    <t>SE350070</t>
-  </si>
-  <si>
-    <t>Dearne and Dove Canal location initially, then moved to the Court House Station.</t>
-  </si>
-  <si>
     <t>Best guess</t>
   </si>
   <si>
-    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.55874&amp;lon=-1.47256&amp;layers=168&amp;b=1</t>
-  </si>
-  <si>
     <t>Peak Forest Canal group</t>
   </si>
   <si>
@@ -543,15 +534,6 @@
     <t>Macclesfield Canal group</t>
   </si>
   <si>
-    <t>SJ940662</t>
-  </si>
-  <si>
-    <t>Top of the hill' comment in 1848 report.</t>
-  </si>
-  <si>
-    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.19330&amp;lon=-2.09051&amp;layers=168&amp;b=1</t>
-  </si>
-  <si>
     <t>Reservoir</t>
   </si>
   <si>
@@ -573,9 +555,6 @@
     <t>Cable Railway Top</t>
   </si>
   <si>
-    <t>SK068803</t>
-  </si>
-  <si>
     <t>Rain Gauge marked on old OS Map at the top of the Peak Forest Tramway's Inclined Plane.</t>
   </si>
   <si>
@@ -597,9 +576,6 @@
     <t>Canal/Wharf then Station</t>
   </si>
   <si>
-    <t>SK387716</t>
-  </si>
-  <si>
     <t>Canal location initially, then moved to the nearby railway station.</t>
   </si>
   <si>
@@ -666,9 +642,6 @@
     <t>SE571036</t>
   </si>
   <si>
-    <t>Don Navigation New Cut location initially, then moved to railway property.</t>
-  </si>
-  <si>
     <t>https://maps.nls.uk/geo/explore/#zoom=18&amp;lat=53.52612&amp;lon=-1.14044&amp;layers=168&amp;b=1</t>
   </si>
   <si>
@@ -786,9 +759,6 @@
     <t>SJ848981</t>
   </si>
   <si>
-    <t>A reference to the canal basin near Piccadilly (street) (by Dulcie Street at the junction with the Rochdale Canal) seems likely.</t>
-  </si>
-  <si>
     <t>https://maps.nls.uk/geo/explore/#zoom=18&amp;lat=53.47971&amp;lon=-2.22958&amp;layers=168&amp;b=1</t>
   </si>
   <si>
@@ -942,9 +912,6 @@
     <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.35555&amp;lon=-1.49078&amp;layers=6&amp;b=1</t>
   </si>
   <si>
-    <t>SK394901</t>
-  </si>
-  <si>
     <t>Tinsley Locks Lock House, on the Sheffield and Tinsley Canal, initially, then moved to a railway location.</t>
   </si>
   <si>
@@ -1006,15 +973,6 @@
   </si>
   <si>
     <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.30693&amp;lon=-1.12273&amp;layers=168&amp;b=1</t>
-  </si>
-  <si>
-    <t>SE353034</t>
-  </si>
-  <si>
-    <t>Worsborough Basin at the end of the Worsborough Branch of the Dearne and Dove Canal</t>
-  </si>
-  <si>
-    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.52664&amp;lon=-1.46830&amp;layers=168&amp;b=1</t>
   </si>
   <si>
     <t>SK299992</t>
@@ -1198,9 +1156,6 @@
     <t>BOLLINGTON-SPONDS-HILL</t>
   </si>
   <si>
-    <t>MARPLE-AQUADUCT</t>
-  </si>
-  <si>
     <t>MOTTRAM-MATTLEYS-FIELD</t>
   </si>
   <si>
@@ -1426,12 +1381,6 @@
     <t>RR415</t>
   </si>
   <si>
-    <t>RR407 ?</t>
-  </si>
-  <si>
-    <t>RR413 ?</t>
-  </si>
-  <si>
     <t>RR162</t>
   </si>
   <si>
@@ -1439,6 +1388,60 @@
   </si>
   <si>
     <t>George Morland Hutton, director of Great Central Railway, lived at Gate Burton. As did his father(?) William Hutton MS&amp;LR director 1864-1874.</t>
+  </si>
+  <si>
+    <t>SE357067</t>
+  </si>
+  <si>
+    <t>SJ931674</t>
+  </si>
+  <si>
+    <t>Dearne and Dove Canal location initially, then moved to the Court House Station. GR is the Lock House at the junction with Barnsley Canal, as one possibility.</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.55738&amp;lon=-1.46320&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>Top of the hill' comment in 1848 report. Gauge shown on map near Bosley Minns seems the likely location.</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.20446&amp;lon=-2.10394&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>SK068802</t>
+  </si>
+  <si>
+    <t>SK386716</t>
+  </si>
+  <si>
+    <t>Don Navigation New Cut location initially, then moved to railway property. GR is Doncaster Town Lock as one possibility</t>
+  </si>
+  <si>
+    <t>MARPLE-AQUEDUCT</t>
+  </si>
+  <si>
+    <t>RR407</t>
+  </si>
+  <si>
+    <t>ROCHDALE [PL]</t>
+  </si>
+  <si>
+    <t>SK394903</t>
+  </si>
+  <si>
+    <t>RR413</t>
+  </si>
+  <si>
+    <t>Worsborough Reservoir Cottage at the end of the Worsborough Branch of the Dearne and Dove Canal</t>
+  </si>
+  <si>
+    <t>SE348035</t>
+  </si>
+  <si>
+    <t>https://maps.nls.uk/geo/explore/#zoom=17&amp;lat=53.52740&amp;lon=-1.47363&amp;layers=168&amp;b=1</t>
+  </si>
+  <si>
+    <t>A reference to the canal basin near Piccadilly (street) (by Dulcie Street at the junction with the Rochdale Canal) seems likely. See https://maps.nls.uk/view/102344087 for early canal course.</t>
   </si>
 </sst>
 </file>
@@ -2706,10 +2709,10 @@
   <dimension ref="A1:S57"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S20" sqref="S20"/>
+      <selection pane="bottomRight" activeCell="R47" sqref="R47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2732,34 +2735,34 @@
         <v>88</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>326</v>
+        <v>312</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>327</v>
+        <v>313</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>328</v>
+        <v>314</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>329</v>
+        <v>315</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>332</v>
+        <v>318</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>334</v>
+        <v>320</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
       <c r="L1" s="3"/>
       <c r="M1" s="9" t="s">
@@ -2772,13 +2775,13 @@
         <v>104</v>
       </c>
       <c r="P1" s="10" t="s">
-        <v>360</v>
+        <v>345</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>361</v>
+        <v>346</v>
       </c>
       <c r="R1" s="114" t="s">
-        <v>362</v>
+        <v>347</v>
       </c>
       <c r="S1" s="3" t="s">
         <v>60</v>
@@ -2820,7 +2823,7 @@
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="7" t="s">
-        <v>302</v>
+        <v>288</v>
       </c>
       <c r="N2" s="7" t="s">
         <v>83</v>
@@ -2832,10 +2835,10 @@
         <v>2</v>
       </c>
       <c r="Q2" t="s">
-        <v>388</v>
+        <v>373</v>
       </c>
       <c r="R2" s="115" t="s">
-        <v>399</v>
+        <v>384</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -2872,7 +2875,7 @@
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="7" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
       <c r="N3" s="7" t="s">
         <v>83</v>
@@ -2887,7 +2890,7 @@
         <v>62</v>
       </c>
       <c r="R3" s="116" t="s">
-        <v>363</v>
+        <v>348</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -2934,10 +2937,10 @@
         <v>2</v>
       </c>
       <c r="Q4" t="s">
-        <v>400</v>
+        <v>385</v>
       </c>
       <c r="R4" s="115" t="s">
-        <v>437</v>
+        <v>420</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -2974,22 +2977,22 @@
       </c>
       <c r="L5" s="3"/>
       <c r="M5" s="7" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
       <c r="N5" s="7" t="s">
         <v>83</v>
       </c>
       <c r="O5" s="17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P5" t="s">
         <v>2</v>
       </c>
       <c r="Q5" s="113" t="s">
-        <v>357</v>
+        <v>343</v>
       </c>
       <c r="R5" s="115" t="s">
-        <v>364</v>
+        <v>349</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -3026,22 +3029,22 @@
       </c>
       <c r="L6" s="3"/>
       <c r="M6" s="7" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
       <c r="N6" s="7" t="s">
         <v>83</v>
       </c>
       <c r="O6" s="17" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="P6" t="s">
         <v>2</v>
       </c>
       <c r="Q6" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="R6" s="116" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -3080,13 +3083,13 @@
       </c>
       <c r="L7" s="3"/>
       <c r="M7" s="7" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="N7" s="7" t="s">
         <v>83</v>
       </c>
       <c r="O7" s="17" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="P7" t="s">
         <v>2</v>
@@ -3095,7 +3098,7 @@
         <v>56</v>
       </c>
       <c r="R7" s="116" t="s">
-        <v>366</v>
+        <v>351</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -3132,7 +3135,7 @@
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="7" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
       <c r="N8" s="7" t="s">
         <v>83</v>
@@ -3147,7 +3150,7 @@
         <v>63</v>
       </c>
       <c r="R8" s="116" t="s">
-        <v>367</v>
+        <v>352</v>
       </c>
       <c r="S8" t="s">
         <v>90</v>
@@ -3189,22 +3192,22 @@
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="7" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
       <c r="N9" s="7" t="s">
         <v>83</v>
       </c>
       <c r="O9" s="17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P9" t="s">
         <v>2</v>
       </c>
       <c r="Q9" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="R9" s="116" t="s">
-        <v>413</v>
+        <v>398</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -3241,16 +3244,16 @@
         <v>83</v>
       </c>
       <c r="O10" s="21" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="P10" t="s">
         <v>3</v>
       </c>
       <c r="Q10" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
       <c r="R10" s="115" t="s">
-        <v>415</v>
+        <v>400</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -3287,27 +3290,27 @@
       </c>
       <c r="L11" s="3"/>
       <c r="M11" s="7" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
       <c r="N11" s="7" t="s">
         <v>83</v>
       </c>
       <c r="O11" s="17" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="P11" t="s">
         <v>2</v>
       </c>
       <c r="Q11" t="s">
-        <v>401</v>
+        <v>386</v>
       </c>
       <c r="R11" s="115" t="s">
-        <v>436</v>
+        <v>419</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B12" s="30"/>
       <c r="C12" s="31">
@@ -3325,13 +3328,13 @@
       </c>
       <c r="L12" s="3"/>
       <c r="M12" s="7" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
       <c r="N12" s="7" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="O12" s="17" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="P12" t="s">
         <v>2</v>
@@ -3376,22 +3379,22 @@
       </c>
       <c r="L13" s="3"/>
       <c r="M13" s="7" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
       <c r="N13" s="7" t="s">
         <v>83</v>
       </c>
       <c r="O13" s="17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P13" t="s">
         <v>2</v>
       </c>
       <c r="Q13" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
       <c r="R13" s="116" t="s">
-        <v>368</v>
+        <v>353</v>
       </c>
       <c r="S13" t="s">
         <v>89</v>
@@ -3427,26 +3430,26 @@
         <v>1</v>
       </c>
       <c r="K14" s="33" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
       <c r="L14" s="3"/>
       <c r="M14" s="7" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
       <c r="N14" s="7" t="s">
         <v>83</v>
       </c>
       <c r="O14" s="17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P14" t="s">
         <v>2</v>
       </c>
       <c r="Q14" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
       <c r="R14" s="116" t="s">
-        <v>369</v>
+        <v>354</v>
       </c>
       <c r="S14" s="6" t="s">
         <v>92</v>
@@ -3496,10 +3499,10 @@
         <v>2</v>
       </c>
       <c r="Q15" t="s">
-        <v>404</v>
+        <v>389</v>
       </c>
       <c r="R15" s="115" t="s">
-        <v>405</v>
+        <v>390</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -3546,10 +3549,10 @@
         <v>2</v>
       </c>
       <c r="Q16" t="s">
-        <v>402</v>
+        <v>387</v>
       </c>
       <c r="R16" s="115" t="s">
-        <v>406</v>
+        <v>391</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
@@ -3586,22 +3589,22 @@
       </c>
       <c r="L17" s="3"/>
       <c r="M17" s="7" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="N17" s="7" t="s">
         <v>83</v>
       </c>
       <c r="O17" s="21" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="P17" t="s">
         <v>3</v>
       </c>
       <c r="Q17" t="s">
-        <v>389</v>
+        <v>374</v>
       </c>
       <c r="R17" s="115" t="s">
-        <v>410</v>
+        <v>395</v>
       </c>
       <c r="S17" t="s">
         <v>93</v>
@@ -3651,10 +3654,10 @@
         <v>2</v>
       </c>
       <c r="Q18" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
       <c r="R18" s="115" t="s">
-        <v>370</v>
+        <v>355</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
@@ -3691,7 +3694,7 @@
       </c>
       <c r="L19" s="3"/>
       <c r="M19" s="7" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
       <c r="N19" s="7" t="s">
         <v>83</v>
@@ -3706,7 +3709,7 @@
         <v>64</v>
       </c>
       <c r="R19" s="116" t="s">
-        <v>371</v>
+        <v>356</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
@@ -3743,7 +3746,7 @@
         <v>84</v>
       </c>
       <c r="O20" s="17" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="P20" t="s">
         <v>2</v>
@@ -3752,7 +3755,7 @@
         <v>101</v>
       </c>
       <c r="R20" s="116" t="s">
-        <v>372</v>
+        <v>357</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
@@ -3789,7 +3792,7 @@
       </c>
       <c r="L21" s="3"/>
       <c r="M21" s="7" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
       <c r="N21" s="7" t="s">
         <v>83</v>
@@ -3804,7 +3807,7 @@
         <v>65</v>
       </c>
       <c r="R21" s="116" t="s">
-        <v>374</v>
+        <v>359</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
@@ -3839,16 +3842,16 @@
         <v>83</v>
       </c>
       <c r="O22" s="17" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="P22" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="Q22" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
       <c r="R22" s="116" t="s">
-        <v>375</v>
+        <v>360</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
@@ -3879,26 +3882,26 @@
         <v>1</v>
       </c>
       <c r="K23" s="33" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="L23" s="3"/>
       <c r="M23" s="7" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="N23" s="7" t="s">
         <v>83</v>
       </c>
       <c r="O23" s="21" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="P23" t="s">
         <v>2</v>
       </c>
       <c r="Q23" t="s">
-        <v>390</v>
+        <v>375</v>
       </c>
       <c r="R23" s="115" t="s">
-        <v>398</v>
+        <v>383</v>
       </c>
       <c r="S23" s="6" t="s">
         <v>94</v>
@@ -3938,7 +3941,7 @@
       </c>
       <c r="L24" s="3"/>
       <c r="M24" s="7" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
       <c r="N24" s="7" t="s">
         <v>83</v>
@@ -3953,7 +3956,7 @@
         <v>66</v>
       </c>
       <c r="R24" s="116" t="s">
-        <v>376</v>
+        <v>361</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
@@ -3990,16 +3993,16 @@
         <v>83</v>
       </c>
       <c r="O25" s="21" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="P25" t="s">
         <v>3</v>
       </c>
       <c r="Q25" t="s">
-        <v>416</v>
+        <v>401</v>
       </c>
       <c r="R25" s="115" t="s">
-        <v>417</v>
+        <v>402</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
@@ -4036,22 +4039,22 @@
       </c>
       <c r="L26" s="3"/>
       <c r="M26" s="7" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
       <c r="N26" s="7" t="s">
         <v>83</v>
       </c>
       <c r="O26" s="17" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="P26" t="s">
         <v>2</v>
       </c>
       <c r="Q26" t="s">
-        <v>391</v>
+        <v>376</v>
       </c>
       <c r="R26" s="115" t="s">
-        <v>397</v>
+        <v>382</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
@@ -4090,7 +4093,7 @@
       </c>
       <c r="L27" s="3"/>
       <c r="M27" s="7" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
       <c r="N27" s="7" t="s">
         <v>83</v>
@@ -4102,10 +4105,10 @@
         <v>2</v>
       </c>
       <c r="Q27" t="s">
-        <v>392</v>
+        <v>377</v>
       </c>
       <c r="R27" s="115" t="s">
-        <v>396</v>
+        <v>381</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
@@ -4142,7 +4145,7 @@
       </c>
       <c r="L28" s="3"/>
       <c r="M28" s="7" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
       <c r="N28" s="7" t="s">
         <v>83</v>
@@ -4154,10 +4157,10 @@
         <v>2</v>
       </c>
       <c r="Q28" t="s">
-        <v>325</v>
+        <v>311</v>
       </c>
       <c r="R28" s="116" t="s">
-        <v>379</v>
+        <v>364</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
@@ -4194,7 +4197,7 @@
       </c>
       <c r="L29" s="3"/>
       <c r="M29" s="7" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
       <c r="N29" s="7" t="s">
         <v>83</v>
@@ -4209,7 +4212,7 @@
         <v>67</v>
       </c>
       <c r="R29" s="116" t="s">
-        <v>377</v>
+        <v>362</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
@@ -4242,22 +4245,22 @@
       </c>
       <c r="L30" s="3"/>
       <c r="M30" s="7" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
       <c r="N30" s="7" t="s">
         <v>85</v>
       </c>
       <c r="O30" s="17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P30" t="s">
         <v>2</v>
       </c>
       <c r="Q30" t="s">
-        <v>358</v>
+        <v>431</v>
       </c>
       <c r="R30" s="115" t="s">
-        <v>380</v>
+        <v>365</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
@@ -4296,13 +4299,13 @@
       </c>
       <c r="L31" s="3"/>
       <c r="M31" s="7" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
       <c r="N31" s="7" t="s">
         <v>83</v>
       </c>
       <c r="O31" s="17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P31" t="s">
         <v>2</v>
@@ -4311,7 +4314,7 @@
         <v>57</v>
       </c>
       <c r="R31" s="116" t="s">
-        <v>381</v>
+        <v>366</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
@@ -4348,16 +4351,16 @@
         <v>86</v>
       </c>
       <c r="O32" s="17" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="P32" t="s">
         <v>2</v>
       </c>
       <c r="Q32" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="R32" s="115" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
@@ -4394,22 +4397,22 @@
       </c>
       <c r="L33" s="3"/>
       <c r="M33" s="7" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
       <c r="N33" s="7" t="s">
         <v>83</v>
       </c>
       <c r="O33" s="21" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="P33" t="s">
         <v>3</v>
       </c>
       <c r="Q33" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="R33" s="115" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="S33" t="s">
         <v>95</v>
@@ -4449,7 +4452,7 @@
       </c>
       <c r="L34" s="3"/>
       <c r="M34" s="7" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
       <c r="N34" s="7" t="s">
         <v>83</v>
@@ -4464,7 +4467,7 @@
         <v>68</v>
       </c>
       <c r="R34" s="116" t="s">
-        <v>378</v>
+        <v>363</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
@@ -4501,13 +4504,13 @@
       </c>
       <c r="L35" s="3"/>
       <c r="M35" s="7" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="N35" s="7" t="s">
         <v>83</v>
       </c>
       <c r="O35" s="21" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="P35" t="s">
         <v>3</v>
@@ -4516,7 +4519,7 @@
         <v>38</v>
       </c>
       <c r="R35" s="116" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
@@ -4553,16 +4556,16 @@
         <v>83</v>
       </c>
       <c r="O36" s="17" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="P36" t="s">
         <v>3</v>
       </c>
       <c r="Q36" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="R36" s="115" t="s">
-        <v>420</v>
+        <v>405</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
@@ -4599,16 +4602,16 @@
         <v>83</v>
       </c>
       <c r="O37" s="21" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="P37" t="s">
         <v>2</v>
       </c>
       <c r="Q37" t="s">
-        <v>421</v>
+        <v>406</v>
       </c>
       <c r="R37" s="115" t="s">
-        <v>422</v>
+        <v>407</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
@@ -4645,13 +4648,13 @@
       </c>
       <c r="L38" s="3"/>
       <c r="M38" s="7" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
       <c r="N38" s="7" t="s">
         <v>83</v>
       </c>
       <c r="O38" s="21" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="P38" t="s">
         <v>3</v>
@@ -4660,7 +4663,7 @@
         <v>61</v>
       </c>
       <c r="R38" s="116" t="s">
-        <v>384</v>
+        <v>369</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
@@ -4697,7 +4700,7 @@
         <v>84</v>
       </c>
       <c r="O39" s="21" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="P39" t="s">
         <v>2</v>
@@ -4706,7 +4709,7 @@
         <v>58</v>
       </c>
       <c r="R39" s="116" t="s">
-        <v>385</v>
+        <v>370</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
@@ -4745,16 +4748,16 @@
         <v>83</v>
       </c>
       <c r="O40" s="21" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="P40" t="s">
         <v>3</v>
       </c>
       <c r="Q40" t="s">
-        <v>423</v>
+        <v>408</v>
       </c>
       <c r="R40" s="115" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
@@ -4791,22 +4794,22 @@
       </c>
       <c r="L41" s="3"/>
       <c r="M41" s="7" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
       <c r="N41" s="7" t="s">
         <v>83</v>
       </c>
       <c r="O41" s="17" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="P41" t="s">
         <v>2</v>
       </c>
       <c r="Q41" t="s">
-        <v>403</v>
+        <v>388</v>
       </c>
       <c r="R41" s="115" t="s">
-        <v>407</v>
+        <v>392</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
@@ -4835,10 +4838,13 @@
         <v>75</v>
       </c>
       <c r="O42" s="17" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="P42" t="s">
         <v>2</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>433</v>
       </c>
       <c r="S42" t="s">
         <v>96</v>
@@ -4913,16 +4919,16 @@
         <v>84</v>
       </c>
       <c r="O44" s="21" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="P44" t="s">
         <v>2</v>
       </c>
       <c r="Q44" t="s">
-        <v>425</v>
+        <v>410</v>
       </c>
       <c r="R44" s="115" t="s">
-        <v>426</v>
+        <v>411</v>
       </c>
       <c r="S44" t="s">
         <v>98</v>
@@ -4970,10 +4976,10 @@
         <v>2</v>
       </c>
       <c r="Q45" t="s">
-        <v>427</v>
+        <v>412</v>
       </c>
       <c r="R45" s="115" t="s">
-        <v>428</v>
+        <v>413</v>
       </c>
       <c r="S45" s="7" t="s">
         <v>99</v>
@@ -5013,22 +5019,22 @@
       </c>
       <c r="L46" s="3"/>
       <c r="M46" s="7" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
       <c r="N46" s="7" t="s">
         <v>83</v>
       </c>
       <c r="O46" s="21" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="P46" t="s">
         <v>3</v>
       </c>
       <c r="Q46" t="s">
-        <v>393</v>
+        <v>378</v>
       </c>
       <c r="R46" s="115" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
       <c r="S46" t="s">
         <v>100</v>
@@ -5068,13 +5074,13 @@
         <v>83</v>
       </c>
       <c r="O47" s="17" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="P47" t="s">
         <v>3</v>
       </c>
       <c r="Q47" t="s">
-        <v>429</v>
+        <v>414</v>
       </c>
       <c r="R47" s="116" t="s">
         <v>435</v>
@@ -5114,13 +5120,13 @@
       </c>
       <c r="L48" s="3"/>
       <c r="M48" s="7" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
       <c r="N48" s="7" t="s">
         <v>83</v>
       </c>
       <c r="O48" s="17" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="P48" t="s">
         <v>2</v>
@@ -5129,7 +5135,7 @@
         <v>102</v>
       </c>
       <c r="R48" s="115" t="s">
-        <v>373</v>
+        <v>358</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
@@ -5166,16 +5172,16 @@
         <v>83</v>
       </c>
       <c r="O49" s="21" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="P49" t="s">
         <v>3</v>
       </c>
       <c r="Q49" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="R49" s="115" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
@@ -5214,19 +5220,19 @@
       </c>
       <c r="L50" s="3"/>
       <c r="M50" s="7" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
       <c r="N50" s="7" t="s">
         <v>83</v>
       </c>
       <c r="O50" s="17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P50" t="s">
         <v>2</v>
       </c>
       <c r="Q50" t="s">
-        <v>394</v>
+        <v>379</v>
       </c>
       <c r="R50" s="115">
         <v>2731</v>
@@ -5268,13 +5274,13 @@
       </c>
       <c r="L51" s="3"/>
       <c r="M51" s="7" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
       <c r="N51" s="7" t="s">
         <v>83</v>
       </c>
       <c r="O51" s="21" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="P51" t="s">
         <v>3</v>
@@ -5283,7 +5289,7 @@
         <v>59</v>
       </c>
       <c r="R51" s="116" t="s">
-        <v>386</v>
+        <v>371</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
@@ -5320,13 +5326,13 @@
       </c>
       <c r="L52" s="3"/>
       <c r="M52" s="7" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
       <c r="N52" s="7" t="s">
         <v>83</v>
       </c>
       <c r="O52" s="17" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="P52" t="s">
         <v>2</v>
@@ -5335,7 +5341,7 @@
         <v>87</v>
       </c>
       <c r="R52" s="116" t="s">
-        <v>387</v>
+        <v>372</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
@@ -5382,10 +5388,10 @@
         <v>2</v>
       </c>
       <c r="Q53" t="s">
-        <v>408</v>
+        <v>393</v>
       </c>
       <c r="R53" s="116" t="s">
-        <v>409</v>
+        <v>394</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
@@ -5422,16 +5428,16 @@
         <v>83</v>
       </c>
       <c r="O54" s="21" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="P54" t="s">
         <v>3</v>
       </c>
       <c r="Q54" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="R54" s="115" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
@@ -5472,11 +5478,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{550385DD-90D9-4324-8AF5-34DA66B6F837}">
   <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I20" sqref="I20"/>
+      <selection pane="bottomRight" activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5622,16 +5628,16 @@
       </c>
       <c r="H4" s="17"/>
       <c r="I4" s="18" t="s">
+        <v>422</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>424</v>
+      </c>
+      <c r="K4" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="J4" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="K4" s="16" t="s">
-        <v>132</v>
-      </c>
       <c r="L4" s="22" t="s">
-        <v>133</v>
+        <v>425</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -5639,7 +5645,7 @@
         <v>37</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C5" s="21">
         <v>1279</v>
@@ -5651,22 +5657,22 @@
         <v>116</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H5" s="17" t="s">
         <v>3</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="K5" s="16" t="s">
         <v>126</v>
       </c>
       <c r="L5" s="22" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -5674,7 +5680,7 @@
         <v>17</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C6" s="21">
         <v>1210</v>
@@ -5686,20 +5692,20 @@
         <v>116</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="H6" s="17"/>
+        <v>132</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>3</v>
+      </c>
       <c r="I6" s="16" t="s">
-        <v>140</v>
+        <v>423</v>
       </c>
       <c r="J6" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="K6" s="16" t="s">
-        <v>132</v>
-      </c>
+        <v>426</v>
+      </c>
+      <c r="K6" s="16"/>
       <c r="L6" s="22" t="s">
-        <v>142</v>
+        <v>427</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -5707,7 +5713,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C7" s="21">
         <v>590</v>
@@ -5719,22 +5725,22 @@
         <v>116</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="H7" s="17" t="s">
         <v>3</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K7" s="16" t="s">
         <v>126</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -5758,14 +5764,14 @@
       </c>
       <c r="H8" s="17"/>
       <c r="I8" s="16" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="J8" s="16"/>
       <c r="K8" s="16" t="s">
         <v>126</v>
       </c>
       <c r="L8" s="22" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -5773,7 +5779,7 @@
         <v>24</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C9" s="21">
         <v>965</v>
@@ -5785,22 +5791,22 @@
         <v>116</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>3</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>150</v>
+        <v>428</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="K9" s="16" t="s">
         <v>126</v>
       </c>
       <c r="L9" s="22" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -5808,7 +5814,7 @@
         <v>43</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C10" s="21">
         <v>84</v>
@@ -5824,12 +5830,12 @@
       </c>
       <c r="H10" s="17"/>
       <c r="I10" s="16" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="J10" s="16"/>
       <c r="K10" s="16"/>
       <c r="L10" s="22" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -5837,7 +5843,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C11" s="21">
         <v>248</v>
@@ -5852,28 +5858,28 @@
         <v>116</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="H11" s="17"/>
       <c r="I11" s="18" t="s">
-        <v>158</v>
+        <v>429</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="L11" s="23" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="C12" s="24" t="s">
         <v>54</v>
@@ -5882,23 +5888,23 @@
         <v>54</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="H12" s="17"/>
       <c r="I12" s="16" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="L12" s="22" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -5906,7 +5912,7 @@
         <v>20</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C13" s="21">
         <v>1669</v>
@@ -5918,22 +5924,22 @@
         <v>116</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H13" s="17" t="s">
         <v>3</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="J13" s="16" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="K13" s="16" t="s">
         <v>126</v>
       </c>
       <c r="L13" s="22" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -5941,7 +5947,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C14" s="21">
         <v>710</v>
@@ -5953,22 +5959,22 @@
         <v>116</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="H14" s="17" t="s">
         <v>3</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="K14" s="16" t="s">
         <v>126</v>
       </c>
       <c r="L14" s="22" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -5991,20 +5997,20 @@
         <v>116</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="H15" s="17"/>
       <c r="I15" s="16" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="J15" s="16" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="L15" s="22" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -6027,20 +6033,20 @@
         <v>116</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="H16" s="17"/>
       <c r="I16" s="16" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="J16" s="16" t="s">
-        <v>181</v>
+        <v>430</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="L16" s="22" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -6048,7 +6054,7 @@
         <v>41</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="C17" s="21">
         <v>954</v>
@@ -6064,14 +6070,14 @@
       </c>
       <c r="H17" s="17"/>
       <c r="I17" s="16" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="J17" s="16"/>
       <c r="K17" s="16" t="s">
         <v>126</v>
       </c>
       <c r="L17" s="22" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -6094,20 +6100,20 @@
         <v>116</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="H18" s="17"/>
       <c r="I18" s="16" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="J18" s="16" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="L18" s="22" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -6131,14 +6137,14 @@
       </c>
       <c r="H19" s="17"/>
       <c r="I19" s="16" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="J19" s="16"/>
       <c r="K19" s="16" t="s">
         <v>126</v>
       </c>
       <c r="L19" s="22" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -6146,7 +6152,7 @@
         <v>22</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="C20" s="21">
         <v>96</v>
@@ -6155,23 +6161,23 @@
         <v>29</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="H20" s="17"/>
       <c r="I20" s="16" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="J20" s="16" t="s">
-        <v>438</v>
+        <v>421</v>
       </c>
       <c r="K20" s="16" t="s">
         <v>126</v>
       </c>
       <c r="L20" s="22" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -6195,16 +6201,16 @@
       </c>
       <c r="H21" s="17"/>
       <c r="I21" s="16" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="J21" s="16" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="K21" s="16" t="s">
         <v>126</v>
       </c>
       <c r="L21" s="22" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -6212,7 +6218,7 @@
         <v>53</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C22" s="21">
         <v>35</v>
@@ -6224,20 +6230,20 @@
         <v>123</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="H22" s="17"/>
       <c r="I22" s="16" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="J22" s="16" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="K22" s="16" t="s">
         <v>126</v>
       </c>
       <c r="L22" s="22" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -6245,7 +6251,7 @@
         <v>36</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C23" s="21">
         <v>238</v>
@@ -6264,16 +6270,16 @@
       </c>
       <c r="H23" s="17"/>
       <c r="I23" s="16" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="K23" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="L23" s="22" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -6297,16 +6303,16 @@
       </c>
       <c r="H24" s="17"/>
       <c r="I24" s="16" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="K24" s="16" t="s">
         <v>126</v>
       </c>
       <c r="L24" s="22" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -6314,7 +6320,7 @@
         <v>45</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C25" s="21">
         <v>40</v>
@@ -6333,16 +6339,16 @@
       </c>
       <c r="H25" s="17"/>
       <c r="I25" s="16" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="J25" s="16" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="K25" s="16" t="s">
         <v>126</v>
       </c>
       <c r="L25" s="22" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -6350,7 +6356,7 @@
         <v>13</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C26" s="21">
         <v>539</v>
@@ -6362,20 +6368,20 @@
         <v>116</v>
       </c>
       <c r="G26" s="16" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="H26" s="17"/>
       <c r="I26" s="16" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="J26" s="16" t="s">
-        <v>411</v>
+        <v>396</v>
       </c>
       <c r="K26" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="L26" s="22" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -6395,20 +6401,20 @@
         <v>116</v>
       </c>
       <c r="G27" s="16" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="H27" s="17"/>
       <c r="I27" s="16" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="J27" s="16" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="K27" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="L27" s="22" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -6428,20 +6434,20 @@
         <v>116</v>
       </c>
       <c r="G28" s="16" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="H28" s="17"/>
       <c r="I28" s="16" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="J28" s="16" t="s">
-        <v>221</v>
+        <v>439</v>
       </c>
       <c r="K28" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="L28" s="22" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -6465,14 +6471,14 @@
       </c>
       <c r="H29" s="17"/>
       <c r="I29" s="16" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="J29" s="16"/>
       <c r="K29" s="16" t="s">
         <v>126</v>
       </c>
       <c r="L29" s="22" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -6480,7 +6486,7 @@
         <v>14</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C30" s="21">
         <v>321</v>
@@ -6492,20 +6498,20 @@
         <v>116</v>
       </c>
       <c r="G30" s="16" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="H30" s="17"/>
       <c r="I30" s="16" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="J30" s="16" t="s">
-        <v>412</v>
+        <v>397</v>
       </c>
       <c r="K30" s="16" t="s">
         <v>126</v>
       </c>
       <c r="L30" s="22" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -6513,7 +6519,7 @@
         <v>26</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C31" s="21">
         <v>543</v>
@@ -6528,20 +6534,20 @@
         <v>116</v>
       </c>
       <c r="G31" s="16" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="H31" s="17"/>
       <c r="I31" s="17" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="J31" s="16" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="K31" s="16" t="s">
         <v>126</v>
       </c>
       <c r="L31" s="22" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -6549,34 +6555,34 @@
         <v>28</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="C32" s="21">
-        <v>600</v>
+        <v>680</v>
       </c>
       <c r="D32" s="21">
+        <v>207</v>
+      </c>
+      <c r="F32" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="F32" s="16" t="s">
-        <v>192</v>
-      </c>
       <c r="G32" s="16" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="H32" s="17" t="s">
         <v>3</v>
       </c>
       <c r="I32" s="16" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="J32" s="16" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="K32" s="16" t="s">
         <v>126</v>
       </c>
       <c r="L32" s="22" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -6584,7 +6590,7 @@
         <v>27</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="C33" s="21">
         <v>399</v>
@@ -6599,22 +6605,22 @@
         <v>123</v>
       </c>
       <c r="G33" s="16" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="H33" s="17" t="s">
         <v>3</v>
       </c>
       <c r="I33" s="16" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="J33" s="16" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="K33" s="16" t="s">
         <v>126</v>
       </c>
       <c r="L33" s="22" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -6640,16 +6646,16 @@
         <v>3</v>
       </c>
       <c r="I34" s="16" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="J34" s="16" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="K34" s="16" t="s">
         <v>126</v>
       </c>
       <c r="L34" s="22" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -6657,7 +6663,7 @@
         <v>15</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="C35" s="24">
         <v>396</v>
@@ -6673,14 +6679,14 @@
       </c>
       <c r="H35" s="17"/>
       <c r="I35" s="16" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="J35" s="16"/>
       <c r="K35" s="16" t="s">
         <v>126</v>
       </c>
       <c r="L35" s="22" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -6688,7 +6694,7 @@
         <v>42</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C36" s="21">
         <v>76</v>
@@ -6704,14 +6710,14 @@
       </c>
       <c r="H36" s="17"/>
       <c r="I36" s="16" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="J36" s="16"/>
       <c r="K36" s="16" t="s">
         <v>126</v>
       </c>
       <c r="L36" s="22" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -6719,7 +6725,7 @@
         <v>47</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C37" s="21">
         <v>553</v>
@@ -6731,20 +6737,20 @@
         <v>123</v>
       </c>
       <c r="G37" s="16" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="H37" s="17"/>
       <c r="I37" s="16" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="J37" s="16" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="K37" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="L37" s="23" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -6752,7 +6758,7 @@
         <v>19</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="C38" s="21">
         <v>717</v>
@@ -6764,20 +6770,20 @@
         <v>123</v>
       </c>
       <c r="G38" s="16" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="H38" s="17"/>
       <c r="I38" s="16" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="J38" s="16" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="K38" s="16" t="s">
         <v>126</v>
       </c>
       <c r="L38" s="22" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -6785,7 +6791,7 @@
         <v>48</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="C39" s="21">
         <v>1075</v>
@@ -6794,23 +6800,23 @@
         <v>328</v>
       </c>
       <c r="F39" s="16" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="G39" s="16" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="H39" s="17"/>
       <c r="I39" s="16" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="J39" s="16" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="K39" s="16" t="s">
         <v>126</v>
       </c>
       <c r="L39" s="22" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -6818,7 +6824,7 @@
         <v>55</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="C40" s="21">
         <v>868</v>
@@ -6834,14 +6840,14 @@
       </c>
       <c r="H40" s="17"/>
       <c r="I40" s="16" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="J40" s="16"/>
       <c r="K40" s="16" t="s">
         <v>126</v>
       </c>
       <c r="L40" s="22" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -6849,7 +6855,7 @@
         <v>1</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C41" s="24">
         <v>52</v>
@@ -6865,16 +6871,16 @@
       </c>
       <c r="H41" s="17"/>
       <c r="I41" s="16" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="J41" s="17" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="K41" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="L41" s="22" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -6882,7 +6888,7 @@
         <v>29</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="C42" s="24" t="s">
         <v>54</v>
@@ -6892,23 +6898,23 @@
       </c>
       <c r="E42" s="24"/>
       <c r="F42" s="16" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="G42" s="16" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="H42" s="17"/>
       <c r="I42" s="17" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="J42" s="16" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="K42" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="L42" s="23" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
@@ -6932,16 +6938,16 @@
       </c>
       <c r="H43" s="17"/>
       <c r="I43" s="16" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="J43" s="16" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="K43" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="L43" s="22" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
@@ -6949,7 +6955,7 @@
         <v>51</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="C44" s="21">
         <v>336</v>
@@ -6958,23 +6964,23 @@
         <v>102</v>
       </c>
       <c r="F44" s="16" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="G44" s="16" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="H44" s="17"/>
       <c r="I44" s="16" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="J44" s="16" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="K44" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="L44" s="22" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -6997,20 +7003,20 @@
         <v>116</v>
       </c>
       <c r="G45" s="16" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="H45" s="17"/>
       <c r="I45" s="16" t="s">
-        <v>273</v>
+        <v>434</v>
       </c>
       <c r="J45" s="16" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="K45" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="L45" s="22" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -7018,7 +7024,7 @@
         <v>52</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="C46" s="24">
         <v>188</v>
@@ -7034,14 +7040,14 @@
       </c>
       <c r="H46" s="17"/>
       <c r="I46" s="16" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="J46" s="16"/>
       <c r="K46" s="16" t="s">
         <v>126</v>
       </c>
       <c r="L46" s="22" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -7049,7 +7055,7 @@
         <v>50</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C47" s="21">
         <v>21</v>
@@ -7065,14 +7071,14 @@
       </c>
       <c r="H47" s="17"/>
       <c r="I47" s="16" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="J47" s="16"/>
       <c r="K47" s="16" t="s">
         <v>126</v>
       </c>
       <c r="L47" s="22" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -7080,7 +7086,7 @@
         <v>9</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C48" s="24">
         <v>21</v>
@@ -7096,16 +7102,16 @@
       </c>
       <c r="H48" s="17"/>
       <c r="I48" s="16" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="J48" s="16" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="K48" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="L48" s="22" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
@@ -7113,7 +7119,7 @@
         <v>44</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C49" s="21">
         <v>59</v>
@@ -7129,14 +7135,14 @@
       </c>
       <c r="H49" s="17"/>
       <c r="I49" s="16" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="J49" s="16"/>
       <c r="K49" s="16" t="s">
         <v>126</v>
       </c>
       <c r="L49" s="22" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -7144,7 +7150,7 @@
         <v>25</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C50" s="24">
         <v>602</v>
@@ -7156,22 +7162,22 @@
         <v>116</v>
       </c>
       <c r="G50" s="16" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="H50" s="17" t="s">
         <v>3</v>
       </c>
       <c r="I50" s="16" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="J50" s="16" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="K50" s="16" t="s">
         <v>126</v>
       </c>
       <c r="L50" s="22" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -7179,7 +7185,7 @@
         <v>21</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="C51" s="21">
         <v>939</v>
@@ -7200,16 +7206,16 @@
         <v>3</v>
       </c>
       <c r="I51" s="16" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="J51" s="16" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="K51" s="16" t="s">
         <v>126</v>
       </c>
       <c r="L51" s="22" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
@@ -7217,7 +7223,7 @@
         <v>10</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C52" s="24">
         <v>127</v>
@@ -7233,16 +7239,16 @@
       </c>
       <c r="H52" s="17"/>
       <c r="I52" s="18" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="J52" s="17" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="K52" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="L52" s="25" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
@@ -7262,20 +7268,20 @@
         <v>116</v>
       </c>
       <c r="G53" s="16" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="H53" s="17"/>
       <c r="I53" s="16" t="s">
-        <v>295</v>
+        <v>437</v>
       </c>
       <c r="J53" s="16" t="s">
-        <v>296</v>
+        <v>436</v>
       </c>
       <c r="K53" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="L53" s="22" t="s">
-        <v>297</v>
+        <v>438</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
@@ -7283,7 +7289,7 @@
         <v>49</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="C54" s="24">
         <v>548</v>
@@ -7298,14 +7304,14 @@
         <v>124</v>
       </c>
       <c r="I54" s="16" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="J54" s="16"/>
       <c r="K54" s="16" t="s">
         <v>126</v>
       </c>
       <c r="L54" s="22" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -7613,57 +7619,54 @@
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1" location="zoom=18&amp;lat=53.50588&amp;lon=-2.12159&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.50588&amp;lon=-2.12159&amp;layers=168&amp;b=1" xr:uid="{9B894C87-2996-47E8-BFEB-A4158F3A85C5}"/>
     <hyperlink ref="L3" r:id="rId2" location="zoom=17&amp;lat=53.57522&amp;lon=-0.41022&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.57522&amp;lon=-0.41022&amp;layers=168&amp;b=1" xr:uid="{3A932460-4663-40F0-BCCE-45984E9F098C}"/>
-    <hyperlink ref="L6" r:id="rId3" location="zoom=17&amp;lat=53.19330&amp;lon=-2.09051&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.19330&amp;lon=-2.09051&amp;layers=168&amp;b=1" xr:uid="{AE9BEDAE-1EB3-4A14-89F2-D512DAEB9FE0}"/>
-    <hyperlink ref="L7" r:id="rId4" location="zoom=17.3&amp;lat=53.18856&amp;lon=-2.10940&amp;layers=168&amp;b=1" xr:uid="{B44C0FDD-E0E1-40EA-9296-FDC8FD1E9D48}"/>
-    <hyperlink ref="L8" r:id="rId5" location="zoom=17&amp;lat=53.54929&amp;lon=-0.48558&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.54929&amp;lon=-0.48558&amp;layers=168&amp;b=1" xr:uid="{E1ED48FB-F1B2-4C9D-824B-10971F78FBB7}"/>
-    <hyperlink ref="L9" r:id="rId6" location="zoom=18&amp;lat=53.31986&amp;lon=-1.89976&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.31986&amp;lon=-1.89976&amp;layers=168&amp;b=1" xr:uid="{69573AD8-B3D0-46EF-A2A0-F5AAD631EF1E}"/>
-    <hyperlink ref="L10" r:id="rId7" location="zoom=18&amp;lat=53.19615&amp;lon=-2.89124&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.19615&amp;lon=-2.89124&amp;layers=168&amp;b=1" xr:uid="{EC1414AB-EA40-4A8E-859B-26AEE9D88C87}"/>
-    <hyperlink ref="L12" r:id="rId8" location="zoom=17&amp;lat=53.30298&amp;lon=-1.93642&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.30298&amp;lon=-1.93642&amp;layers=168&amp;b=1" xr:uid="{2A912195-2A8B-4051-B2A6-FC0BF7A51131}"/>
-    <hyperlink ref="L13" r:id="rId9" location="zoom=17&amp;lat=53.28409&amp;lon=-1.91222&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.28409&amp;lon=-1.91222&amp;layers=168&amp;b=1" xr:uid="{CCC042EE-2A34-4B58-8B5A-9906BCA88910}"/>
-    <hyperlink ref="L14" r:id="rId10" location="zoom=17&amp;lat=53.31647&amp;lon=-1.94818&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.31647&amp;lon=-1.94818&amp;layers=168&amp;b=1" xr:uid="{8BB2F39F-774C-4587-B7E0-61FFEDD3BD86}"/>
-    <hyperlink ref="L15" r:id="rId11" location="zoom=17&amp;lat=53.59318&amp;lon=-0.74130&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.59318&amp;lon=-0.74130&amp;layers=168&amp;b=1" xr:uid="{23BFDB11-7F7A-4197-960C-583EC17258E6}"/>
-    <hyperlink ref="L16" r:id="rId12" location="zoom=18&amp;lat=53.52612&amp;lon=-1.14044&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.52612&amp;lon=-1.14044&amp;layers=168&amp;b=1" xr:uid="{C416CD5F-BC4A-42E7-93C6-C94B65BFDF69}"/>
-    <hyperlink ref="L17" r:id="rId13" location="zoom=17&amp;lat=53.51758&amp;lon=-1.76333&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.51758&amp;lon=-1.76333&amp;layers=168&amp;b=1" xr:uid="{8EA5B3C4-FF54-4C32-A3DF-A30A81A254BA}"/>
-    <hyperlink ref="L18" r:id="rId14" location="zoom=18&amp;lat=53.49631&amp;lon=-1.41723&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.49631&amp;lon=-1.41723&amp;layers=168&amp;b=1" xr:uid="{E29FDE03-0E45-4938-955A-A08048B63E60}"/>
-    <hyperlink ref="L19" r:id="rId15" location="zoom=17&amp;lat=53.39956&amp;lon=-0.76993&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.39956&amp;lon=-0.76993&amp;layers=168&amp;b=1" xr:uid="{61ECAA8D-2931-4259-AD81-838456189860}"/>
-    <hyperlink ref="L20" r:id="rId16" location="zoom=17&amp;lat=53.34037&amp;lon=-0.73761&amp;layers=168&amp;b=1" display="zoom=17&amp;lat=53.34037&amp;lon=-0.73761&amp;layers=168&amp;b=1" xr:uid="{DB0067B6-CE6C-4EDC-B07C-D26E94C62F80}"/>
-    <hyperlink ref="L21" r:id="rId17" location="zoom=17&amp;lat=53.56367&amp;lon=-0.08679&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.56367&amp;lon=-0.08679&amp;layers=168&amp;b=1" xr:uid="{8B0420BE-BD8A-4321-BD82-B6F59BC35D5A}"/>
-    <hyperlink ref="L22" r:id="rId18" location="zoom=17&amp;lat=53.21750&amp;lon=-3.03250&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.21750&amp;lon=-3.03250&amp;layers=168&amp;b=1" xr:uid="{A5BA297F-B48F-41E7-A307-1D46476C6A36}"/>
-    <hyperlink ref="L23" r:id="rId19" location="zoom=17&amp;lat=53.33352&amp;lon=-1.29263&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.33352&amp;lon=-1.29263&amp;layers=168&amp;b=1" xr:uid="{943F15D6-2EDC-44DA-956C-C273B35A9FDC}"/>
-    <hyperlink ref="L24" r:id="rId20" location="zoom=17&amp;lat=53.22522&amp;lon=-0.54299&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.22522&amp;lon=-0.54299&amp;layers=168&amp;b=1" xr:uid="{C791D758-1DDF-4AA4-B40A-7FD8D6D74891}"/>
-    <hyperlink ref="L25" r:id="rId21" location="zoom=17&amp;lat=53.42881&amp;lon=-2.99018&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.42881&amp;lon=-2.99018&amp;layers=168&amp;b=1" xr:uid="{79BF8551-6673-4418-83FA-D4F7467E5671}"/>
-    <hyperlink ref="L26" r:id="rId22" location="zoom=18&amp;lat=53.25188&amp;lon=-2.11476&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.25188&amp;lon=-2.11476&amp;layers=168&amp;b=1" xr:uid="{7A36BB20-7096-4776-B194-41081EFD76F1}"/>
-    <hyperlink ref="L27" r:id="rId23" location="zoom=18&amp;lat=53.47779&amp;lon=-2.14979&amp;layers=168&amp;b=1" display="zoom=18&amp;lat=53.47779&amp;lon=-2.14979&amp;layers=168&amp;b=1" xr:uid="{1A68EFEB-3479-41E4-A6F1-45BBB485D43D}"/>
-    <hyperlink ref="L28" r:id="rId24" location="zoom=18&amp;lat=53.47971&amp;lon=-2.22958&amp;layers=168&amp;b=1" display="zoom=18&amp;lat=53.47971&amp;lon=-2.22958&amp;layers=168&amp;b=1" xr:uid="{7E0ACDA6-FAC8-4CDF-8FDD-5DB0B7C90DE1}"/>
-    <hyperlink ref="L29" r:id="rId25" location="zoom=17&amp;lat=53.38440&amp;lon=-0.33806&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.38440&amp;lon=-0.33806&amp;layers=168&amp;b=1" xr:uid="{95B84890-817E-4C65-9F82-C6376DD7E76C}"/>
-    <hyperlink ref="L30" r:id="rId26" location="zoom=18&amp;lat=53.40755&amp;lon=-2.06899&amp;layers=168&amp;b=1" xr:uid="{A9088DEA-9D72-4279-ACE6-4579AAC6255C}"/>
-    <hyperlink ref="L31" r:id="rId27" location="zoom=18&amp;lat=53.39283&amp;lon=-2.05947&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.39283&amp;lon=-2.05947&amp;layers=168&amp;b=1" xr:uid="{88357CC2-F767-41C5-9F18-47CFE5575D14}"/>
-    <hyperlink ref="L32" r:id="rId28" location="zoom=17&amp;lat=53.44610&amp;lon=-2.01568&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.44610&amp;lon=-2.01568&amp;layers=168&amp;b=1" xr:uid="{482E9D44-1BBC-4622-BF55-2280C82C4F69}"/>
-    <hyperlink ref="L33" r:id="rId29" location="zoom=18&amp;lat=53.44067&amp;lon=-2.01577&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.44067&amp;lon=-2.01577&amp;layers=168&amp;b=1" xr:uid="{E6603135-7879-4BA2-8FD7-469042B7E7E0}"/>
-    <hyperlink ref="L34" r:id="rId30" location="zoom=17&amp;lat=53.70469&amp;lon=-0.36412&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.70469&amp;lon=-0.36412&amp;layers=168&amp;b=1" xr:uid="{B807B8F4-E8EC-4E79-8C4B-4D5A93676033}"/>
-    <hyperlink ref="L35" r:id="rId31" location="zoom=18&amp;lat=53.45685&amp;lon=-2.06718&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.45685&amp;lon=-2.06718&amp;layers=168&amp;b=1" xr:uid="{A4F7F856-C870-4CA7-B810-81E0AC9BE366}"/>
-    <hyperlink ref="L36" r:id="rId32" location="zoom=17&amp;lat=53.26174&amp;lon=-2.49629&amp;layers=168&amp;b=1" display="zoom=17&amp;lat=53.26174&amp;lon=-2.49629&amp;layers=168&amp;b=1" xr:uid="{2D008E1F-4F05-4DC6-BA0E-90CA76AE9A33}"/>
-    <hyperlink ref="L38" r:id="rId33" location="zoom=18&amp;lat=53.52679&amp;lon=-1.63269&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.52679&amp;lon=-1.63269&amp;layers=168&amp;b=1" xr:uid="{5D178EE7-846E-4823-BEB5-5F0EFCFB1BD2}"/>
-    <hyperlink ref="L39" r:id="rId34" location="zoom=17&amp;lat=53.52618&amp;lon=-1.73224&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.52618&amp;lon=-1.73224&amp;layers=168&amp;b=1" xr:uid="{24F3EC29-7181-4A9B-9C5A-645FB433FFFE}"/>
-    <hyperlink ref="L40" r:id="rId35" location="zoom=18&amp;lat=53.52204&amp;lon=-1.70992&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.52204&amp;lon=-1.70992&amp;layers=168&amp;b=1" xr:uid="{27FB78A1-2CCA-4977-A322-BAD43ACE9E53}"/>
-    <hyperlink ref="L41" r:id="rId36" location="zoom=18&amp;lat=53.31880&amp;lon=-0.94143&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.31880&amp;lon=-0.94143&amp;layers=168&amp;b=1" xr:uid="{07123CEC-0031-42D2-ACE3-0A88DBC43A06}"/>
-    <hyperlink ref="L43" r:id="rId37" location="zoom=18&amp;lat=53.43074&amp;lon=-1.36062&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.43074&amp;lon=-1.36062&amp;layers=168&amp;b=1" xr:uid="{8A6AAC25-81AA-42AE-B8DD-0F632B56CE52}"/>
-    <hyperlink ref="L44" r:id="rId38" location="zoom=17&amp;lat=53.35555&amp;lon=-1.49078&amp;layers=6&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.35555&amp;lon=-1.49078&amp;layers=6&amp;b=1" xr:uid="{725A1FD7-B475-44EB-87AD-C93D5DE6151C}"/>
-    <hyperlink ref="L45" r:id="rId39" location="zoom=17&amp;lat=53.40626&amp;lon=-1.41062&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.40626&amp;lon=-1.41062&amp;layers=168&amp;b=1" xr:uid="{99F52E2A-9C75-42D9-B4C0-B1E8EB51E551}"/>
-    <hyperlink ref="L46" r:id="rId40" location="zoom=18&amp;lat=53.38769&amp;lon=-1.45865&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.38769&amp;lon=-1.45865&amp;layers=168&amp;b=1" xr:uid="{CEA44F0C-5B20-42C1-8DB8-D1CC7364EAA8}"/>
-    <hyperlink ref="L47" r:id="rId41" location="zoom=17&amp;lat=53.64571&amp;lon=-3.01232&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.64571&amp;lon=-3.01232&amp;layers=168&amp;b=1" xr:uid="{2B777C52-618D-42DC-A42C-51C45B3215FB}"/>
-    <hyperlink ref="L48" r:id="rId42" location="zoom=17&amp;lat=53.44300&amp;lon=-0.81993&amp;layers=168&amp;b=1" xr:uid="{96C4AD99-4E35-403D-A1CB-D53CE39CADBB}"/>
-    <hyperlink ref="L49" r:id="rId43" location="zoom=18&amp;lat=53.39228&amp;lon=-2.59245&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.39228&amp;lon=-2.59245&amp;layers=168&amp;b=1" xr:uid="{A385F51F-D7E6-44E8-B23A-08B45395411F}"/>
-    <hyperlink ref="L50" r:id="rId44" location="zoom=18&amp;lat=53.32784&amp;lon=-1.99017&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.32784&amp;lon=-1.99017&amp;layers=168&amp;b=1" xr:uid="{BBC7B1FD-E213-4B2D-9994-24234CDD4C28}"/>
-    <hyperlink ref="L51" r:id="rId45" location="zoom=18&amp;lat=53.49567&amp;lon=-1.83280&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.49567&amp;lon=-1.83280&amp;layers=168&amp;b=1" xr:uid="{8830D605-CD67-4E77-9DC3-A108B5D718FC}"/>
-    <hyperlink ref="L53" r:id="rId46" location="zoom=17&amp;lat=53.52664&amp;lon=-1.46830&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.52664&amp;lon=-1.46830&amp;layers=168&amp;b=1" xr:uid="{DA5F610B-1D5B-42E9-9721-0981C0544540}"/>
-    <hyperlink ref="L54" r:id="rId47" location="zoom=18&amp;lat=53.48849&amp;lon=-1.55083&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.48849&amp;lon=-1.55083&amp;layers=168&amp;b=1" xr:uid="{5B27AED8-71AA-46F6-8579-50F87BA43DE9}"/>
-    <hyperlink ref="L37" r:id="rId48" location="zoom=17&amp;lat=53.53026&amp;lon=-2.10362&amp;layers=168&amp;b=1" display="zoom=17&amp;lat=53.53026&amp;lon=-2.10362&amp;layers=168&amp;b=1" xr:uid="{5CE0239F-60FA-418E-8E2C-4F9A6FCB5B45}"/>
-    <hyperlink ref="L11" r:id="rId49" location="zoom=17&amp;lat=53.24038&amp;lon=-1.42144&amp;layers=168&amp;b=1" display="zoom=17&amp;lat=53.24038&amp;lon=-1.42144&amp;layers=168&amp;b=1" xr:uid="{4003A536-3F5A-450E-9AD8-9412E92B6060}"/>
-    <hyperlink ref="L52" r:id="rId50" location="zoom=17&amp;lat=53.30693&amp;lon=-1.12273&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.30693&amp;lon=-1.12273&amp;layers=168&amp;b=1" xr:uid="{C5CDAA38-1C18-48A6-AA11-FA85024A4DBB}"/>
-    <hyperlink ref="L42" r:id="rId51" location="zoom=17&amp;lat=53.61390&amp;lon=-2.15339&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.61390&amp;lon=-2.15339&amp;layers=168&amp;b=1" xr:uid="{F4068E9A-645F-424D-8BC0-7CC7F951F71F}"/>
-    <hyperlink ref="L5" r:id="rId52" location="zoom=17&amp;lat=53.31096&amp;lon=-2.04655&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.31096&amp;lon=-2.04655&amp;layers=168&amp;b=1" xr:uid="{F8D79F54-755B-4146-8981-12372D166779}"/>
-    <hyperlink ref="L4" r:id="rId53" location="zoom=17&amp;lat=53.55874&amp;lon=-1.47256&amp;layers=168&amp;b=1" xr:uid="{AFFAACBF-E426-4EFE-8807-1164163FA162}"/>
+    <hyperlink ref="L7" r:id="rId3" location="zoom=17.3&amp;lat=53.18856&amp;lon=-2.10940&amp;layers=168&amp;b=1" xr:uid="{B44C0FDD-E0E1-40EA-9296-FDC8FD1E9D48}"/>
+    <hyperlink ref="L8" r:id="rId4" location="zoom=17&amp;lat=53.54929&amp;lon=-0.48558&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.54929&amp;lon=-0.48558&amp;layers=168&amp;b=1" xr:uid="{E1ED48FB-F1B2-4C9D-824B-10971F78FBB7}"/>
+    <hyperlink ref="L9" r:id="rId5" location="zoom=18&amp;lat=53.31986&amp;lon=-1.89976&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.31986&amp;lon=-1.89976&amp;layers=168&amp;b=1" xr:uid="{69573AD8-B3D0-46EF-A2A0-F5AAD631EF1E}"/>
+    <hyperlink ref="L10" r:id="rId6" location="zoom=18&amp;lat=53.19615&amp;lon=-2.89124&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.19615&amp;lon=-2.89124&amp;layers=168&amp;b=1" xr:uid="{EC1414AB-EA40-4A8E-859B-26AEE9D88C87}"/>
+    <hyperlink ref="L12" r:id="rId7" location="zoom=17&amp;lat=53.30298&amp;lon=-1.93642&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.30298&amp;lon=-1.93642&amp;layers=168&amp;b=1" xr:uid="{2A912195-2A8B-4051-B2A6-FC0BF7A51131}"/>
+    <hyperlink ref="L13" r:id="rId8" location="zoom=17&amp;lat=53.28409&amp;lon=-1.91222&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.28409&amp;lon=-1.91222&amp;layers=168&amp;b=1" xr:uid="{CCC042EE-2A34-4B58-8B5A-9906BCA88910}"/>
+    <hyperlink ref="L14" r:id="rId9" location="zoom=17&amp;lat=53.31647&amp;lon=-1.94818&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.31647&amp;lon=-1.94818&amp;layers=168&amp;b=1" xr:uid="{8BB2F39F-774C-4587-B7E0-61FFEDD3BD86}"/>
+    <hyperlink ref="L15" r:id="rId10" location="zoom=17&amp;lat=53.59318&amp;lon=-0.74130&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.59318&amp;lon=-0.74130&amp;layers=168&amp;b=1" xr:uid="{23BFDB11-7F7A-4197-960C-583EC17258E6}"/>
+    <hyperlink ref="L16" r:id="rId11" location="zoom=18&amp;lat=53.52612&amp;lon=-1.14044&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.52612&amp;lon=-1.14044&amp;layers=168&amp;b=1" xr:uid="{C416CD5F-BC4A-42E7-93C6-C94B65BFDF69}"/>
+    <hyperlink ref="L17" r:id="rId12" location="zoom=17&amp;lat=53.51758&amp;lon=-1.76333&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.51758&amp;lon=-1.76333&amp;layers=168&amp;b=1" xr:uid="{8EA5B3C4-FF54-4C32-A3DF-A30A81A254BA}"/>
+    <hyperlink ref="L18" r:id="rId13" location="zoom=18&amp;lat=53.49631&amp;lon=-1.41723&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.49631&amp;lon=-1.41723&amp;layers=168&amp;b=1" xr:uid="{E29FDE03-0E45-4938-955A-A08048B63E60}"/>
+    <hyperlink ref="L19" r:id="rId14" location="zoom=17&amp;lat=53.39956&amp;lon=-0.76993&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.39956&amp;lon=-0.76993&amp;layers=168&amp;b=1" xr:uid="{61ECAA8D-2931-4259-AD81-838456189860}"/>
+    <hyperlink ref="L20" r:id="rId15" location="zoom=17&amp;lat=53.34037&amp;lon=-0.73761&amp;layers=168&amp;b=1" display="zoom=17&amp;lat=53.34037&amp;lon=-0.73761&amp;layers=168&amp;b=1" xr:uid="{DB0067B6-CE6C-4EDC-B07C-D26E94C62F80}"/>
+    <hyperlink ref="L21" r:id="rId16" location="zoom=17&amp;lat=53.56367&amp;lon=-0.08679&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.56367&amp;lon=-0.08679&amp;layers=168&amp;b=1" xr:uid="{8B0420BE-BD8A-4321-BD82-B6F59BC35D5A}"/>
+    <hyperlink ref="L22" r:id="rId17" location="zoom=17&amp;lat=53.21750&amp;lon=-3.03250&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.21750&amp;lon=-3.03250&amp;layers=168&amp;b=1" xr:uid="{A5BA297F-B48F-41E7-A307-1D46476C6A36}"/>
+    <hyperlink ref="L23" r:id="rId18" location="zoom=17&amp;lat=53.33352&amp;lon=-1.29263&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.33352&amp;lon=-1.29263&amp;layers=168&amp;b=1" xr:uid="{943F15D6-2EDC-44DA-956C-C273B35A9FDC}"/>
+    <hyperlink ref="L24" r:id="rId19" location="zoom=17&amp;lat=53.22522&amp;lon=-0.54299&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.22522&amp;lon=-0.54299&amp;layers=168&amp;b=1" xr:uid="{C791D758-1DDF-4AA4-B40A-7FD8D6D74891}"/>
+    <hyperlink ref="L25" r:id="rId20" location="zoom=17&amp;lat=53.42881&amp;lon=-2.99018&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.42881&amp;lon=-2.99018&amp;layers=168&amp;b=1" xr:uid="{79BF8551-6673-4418-83FA-D4F7467E5671}"/>
+    <hyperlink ref="L26" r:id="rId21" location="zoom=18&amp;lat=53.25188&amp;lon=-2.11476&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.25188&amp;lon=-2.11476&amp;layers=168&amp;b=1" xr:uid="{7A36BB20-7096-4776-B194-41081EFD76F1}"/>
+    <hyperlink ref="L27" r:id="rId22" location="zoom=18&amp;lat=53.47779&amp;lon=-2.14979&amp;layers=168&amp;b=1" display="zoom=18&amp;lat=53.47779&amp;lon=-2.14979&amp;layers=168&amp;b=1" xr:uid="{1A68EFEB-3479-41E4-A6F1-45BBB485D43D}"/>
+    <hyperlink ref="L28" r:id="rId23" location="zoom=18&amp;lat=53.47971&amp;lon=-2.22958&amp;layers=168&amp;b=1" display="zoom=18&amp;lat=53.47971&amp;lon=-2.22958&amp;layers=168&amp;b=1" xr:uid="{7E0ACDA6-FAC8-4CDF-8FDD-5DB0B7C90DE1}"/>
+    <hyperlink ref="L29" r:id="rId24" location="zoom=17&amp;lat=53.38440&amp;lon=-0.33806&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.38440&amp;lon=-0.33806&amp;layers=168&amp;b=1" xr:uid="{95B84890-817E-4C65-9F82-C6376DD7E76C}"/>
+    <hyperlink ref="L30" r:id="rId25" location="zoom=18&amp;lat=53.40755&amp;lon=-2.06899&amp;layers=168&amp;b=1" xr:uid="{A9088DEA-9D72-4279-ACE6-4579AAC6255C}"/>
+    <hyperlink ref="L31" r:id="rId26" location="zoom=18&amp;lat=53.39283&amp;lon=-2.05947&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.39283&amp;lon=-2.05947&amp;layers=168&amp;b=1" xr:uid="{88357CC2-F767-41C5-9F18-47CFE5575D14}"/>
+    <hyperlink ref="L32" r:id="rId27" location="zoom=17&amp;lat=53.44610&amp;lon=-2.01568&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.44610&amp;lon=-2.01568&amp;layers=168&amp;b=1" xr:uid="{482E9D44-1BBC-4622-BF55-2280C82C4F69}"/>
+    <hyperlink ref="L33" r:id="rId28" location="zoom=18&amp;lat=53.44067&amp;lon=-2.01577&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.44067&amp;lon=-2.01577&amp;layers=168&amp;b=1" xr:uid="{E6603135-7879-4BA2-8FD7-469042B7E7E0}"/>
+    <hyperlink ref="L34" r:id="rId29" location="zoom=17&amp;lat=53.70469&amp;lon=-0.36412&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.70469&amp;lon=-0.36412&amp;layers=168&amp;b=1" xr:uid="{B807B8F4-E8EC-4E79-8C4B-4D5A93676033}"/>
+    <hyperlink ref="L35" r:id="rId30" location="zoom=18&amp;lat=53.45685&amp;lon=-2.06718&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.45685&amp;lon=-2.06718&amp;layers=168&amp;b=1" xr:uid="{A4F7F856-C870-4CA7-B810-81E0AC9BE366}"/>
+    <hyperlink ref="L36" r:id="rId31" location="zoom=17&amp;lat=53.26174&amp;lon=-2.49629&amp;layers=168&amp;b=1" display="zoom=17&amp;lat=53.26174&amp;lon=-2.49629&amp;layers=168&amp;b=1" xr:uid="{2D008E1F-4F05-4DC6-BA0E-90CA76AE9A33}"/>
+    <hyperlink ref="L38" r:id="rId32" location="zoom=18&amp;lat=53.52679&amp;lon=-1.63269&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.52679&amp;lon=-1.63269&amp;layers=168&amp;b=1" xr:uid="{5D178EE7-846E-4823-BEB5-5F0EFCFB1BD2}"/>
+    <hyperlink ref="L39" r:id="rId33" location="zoom=17&amp;lat=53.52618&amp;lon=-1.73224&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.52618&amp;lon=-1.73224&amp;layers=168&amp;b=1" xr:uid="{24F3EC29-7181-4A9B-9C5A-645FB433FFFE}"/>
+    <hyperlink ref="L40" r:id="rId34" location="zoom=18&amp;lat=53.52204&amp;lon=-1.70992&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.52204&amp;lon=-1.70992&amp;layers=168&amp;b=1" xr:uid="{27FB78A1-2CCA-4977-A322-BAD43ACE9E53}"/>
+    <hyperlink ref="L41" r:id="rId35" location="zoom=18&amp;lat=53.31880&amp;lon=-0.94143&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.31880&amp;lon=-0.94143&amp;layers=168&amp;b=1" xr:uid="{07123CEC-0031-42D2-ACE3-0A88DBC43A06}"/>
+    <hyperlink ref="L43" r:id="rId36" location="zoom=18&amp;lat=53.43074&amp;lon=-1.36062&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.43074&amp;lon=-1.36062&amp;layers=168&amp;b=1" xr:uid="{8A6AAC25-81AA-42AE-B8DD-0F632B56CE52}"/>
+    <hyperlink ref="L44" r:id="rId37" location="zoom=17&amp;lat=53.35555&amp;lon=-1.49078&amp;layers=6&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.35555&amp;lon=-1.49078&amp;layers=6&amp;b=1" xr:uid="{725A1FD7-B475-44EB-87AD-C93D5DE6151C}"/>
+    <hyperlink ref="L45" r:id="rId38" location="zoom=17&amp;lat=53.40626&amp;lon=-1.41062&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.40626&amp;lon=-1.41062&amp;layers=168&amp;b=1" xr:uid="{99F52E2A-9C75-42D9-B4C0-B1E8EB51E551}"/>
+    <hyperlink ref="L46" r:id="rId39" location="zoom=18&amp;lat=53.38769&amp;lon=-1.45865&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.38769&amp;lon=-1.45865&amp;layers=168&amp;b=1" xr:uid="{CEA44F0C-5B20-42C1-8DB8-D1CC7364EAA8}"/>
+    <hyperlink ref="L47" r:id="rId40" location="zoom=17&amp;lat=53.64571&amp;lon=-3.01232&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.64571&amp;lon=-3.01232&amp;layers=168&amp;b=1" xr:uid="{2B777C52-618D-42DC-A42C-51C45B3215FB}"/>
+    <hyperlink ref="L48" r:id="rId41" location="zoom=17&amp;lat=53.44300&amp;lon=-0.81993&amp;layers=168&amp;b=1" xr:uid="{96C4AD99-4E35-403D-A1CB-D53CE39CADBB}"/>
+    <hyperlink ref="L49" r:id="rId42" location="zoom=18&amp;lat=53.39228&amp;lon=-2.59245&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.39228&amp;lon=-2.59245&amp;layers=168&amp;b=1" xr:uid="{A385F51F-D7E6-44E8-B23A-08B45395411F}"/>
+    <hyperlink ref="L50" r:id="rId43" location="zoom=18&amp;lat=53.32784&amp;lon=-1.99017&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.32784&amp;lon=-1.99017&amp;layers=168&amp;b=1" xr:uid="{BBC7B1FD-E213-4B2D-9994-24234CDD4C28}"/>
+    <hyperlink ref="L51" r:id="rId44" location="zoom=18&amp;lat=53.49567&amp;lon=-1.83280&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.49567&amp;lon=-1.83280&amp;layers=168&amp;b=1" xr:uid="{8830D605-CD67-4E77-9DC3-A108B5D718FC}"/>
+    <hyperlink ref="L54" r:id="rId45" location="zoom=18&amp;lat=53.48849&amp;lon=-1.55083&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=18&amp;lat=53.48849&amp;lon=-1.55083&amp;layers=168&amp;b=1" xr:uid="{5B27AED8-71AA-46F6-8579-50F87BA43DE9}"/>
+    <hyperlink ref="L37" r:id="rId46" location="zoom=17&amp;lat=53.53026&amp;lon=-2.10362&amp;layers=168&amp;b=1" display="zoom=17&amp;lat=53.53026&amp;lon=-2.10362&amp;layers=168&amp;b=1" xr:uid="{5CE0239F-60FA-418E-8E2C-4F9A6FCB5B45}"/>
+    <hyperlink ref="L11" r:id="rId47" location="zoom=17&amp;lat=53.24038&amp;lon=-1.42144&amp;layers=168&amp;b=1" display="zoom=17&amp;lat=53.24038&amp;lon=-1.42144&amp;layers=168&amp;b=1" xr:uid="{4003A536-3F5A-450E-9AD8-9412E92B6060}"/>
+    <hyperlink ref="L52" r:id="rId48" location="zoom=17&amp;lat=53.30693&amp;lon=-1.12273&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.30693&amp;lon=-1.12273&amp;layers=168&amp;b=1" xr:uid="{C5CDAA38-1C18-48A6-AA11-FA85024A4DBB}"/>
+    <hyperlink ref="L42" r:id="rId49" location="zoom=17&amp;lat=53.61390&amp;lon=-2.15339&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.61390&amp;lon=-2.15339&amp;layers=168&amp;b=1" xr:uid="{F4068E9A-645F-424D-8BC0-7CC7F951F71F}"/>
+    <hyperlink ref="L5" r:id="rId50" location="zoom=17&amp;lat=53.31096&amp;lon=-2.04655&amp;layers=168&amp;b=1" display="https://maps.nls.uk/geo/explore/ - zoom=17&amp;lat=53.31096&amp;lon=-2.04655&amp;layers=168&amp;b=1" xr:uid="{F8D79F54-755B-4146-8981-12372D166779}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7673,11 +7676,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7272480D-31B6-4325-B44F-959F48A55EA8}">
   <dimension ref="A1:CN92"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="E39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="AT68" sqref="AT68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7693,57 +7696,57 @@
     <row r="1" spans="1:92" ht="21" x14ac:dyDescent="0.35">
       <c r="F1" s="34"/>
       <c r="J1" s="36" t="s">
-        <v>326</v>
+        <v>312</v>
       </c>
       <c r="O1" s="37"/>
       <c r="P1" s="34"/>
       <c r="T1" s="36" t="s">
-        <v>327</v>
+        <v>313</v>
       </c>
       <c r="Y1" s="37"/>
       <c r="Z1" s="34"/>
       <c r="AD1" s="36" t="s">
-        <v>328</v>
+        <v>314</v>
       </c>
       <c r="AI1" s="37"/>
       <c r="AJ1" s="34"/>
       <c r="AN1" s="36" t="s">
-        <v>329</v>
+        <v>315</v>
       </c>
       <c r="AS1" s="37"/>
       <c r="AT1" s="34"/>
       <c r="AX1" s="36" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
       <c r="BC1" s="37"/>
       <c r="BD1" s="34"/>
       <c r="BH1" s="36" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
       <c r="BM1" s="38"/>
       <c r="BR1" s="36" t="s">
-        <v>332</v>
+        <v>318</v>
       </c>
       <c r="BW1" s="37"/>
       <c r="BX1" s="34"/>
       <c r="CB1" s="36" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
       <c r="CG1" s="39"/>
       <c r="CJ1" s="40"/>
       <c r="CL1" s="36" t="s">
-        <v>334</v>
+        <v>320</v>
       </c>
     </row>
     <row r="2" spans="1:92" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="41" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>336</v>
+        <v>322</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>337</v>
+        <v>323</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>104</v>
@@ -8007,7 +8010,7 @@
         <v>1925</v>
       </c>
       <c r="CN2" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
     </row>
     <row r="3" spans="1:92" x14ac:dyDescent="0.25">
@@ -8104,12 +8107,12 @@
     </row>
     <row r="4" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
-        <v>339</v>
+        <v>325</v>
       </c>
       <c r="B4" s="48"/>
       <c r="C4" s="48"/>
       <c r="D4" s="49" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="F4" s="42"/>
       <c r="G4" s="50"/>
@@ -8200,12 +8203,12 @@
     </row>
     <row r="5" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
-        <v>341</v>
+        <v>327</v>
       </c>
       <c r="B5" s="48"/>
       <c r="C5" s="48"/>
       <c r="D5" s="49" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="F5" s="42"/>
       <c r="G5" s="43"/>
@@ -8296,12 +8299,12 @@
     </row>
     <row r="6" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A6" s="47" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
       <c r="B6" s="48"/>
       <c r="C6" s="48"/>
       <c r="D6" s="49" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="F6" s="42"/>
       <c r="G6" s="43"/>
@@ -8392,12 +8395,12 @@
     </row>
     <row r="7" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A7" s="47" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
       <c r="B7" s="48"/>
       <c r="C7" s="48"/>
       <c r="D7" s="49" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="F7" s="42"/>
       <c r="G7" s="43"/>
@@ -8488,12 +8491,12 @@
     </row>
     <row r="8" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A8" s="47" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
       <c r="B8" s="48"/>
       <c r="C8" s="48"/>
       <c r="D8" s="49" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="F8" s="42"/>
       <c r="G8" s="43"/>
@@ -8584,12 +8587,12 @@
     </row>
     <row r="9" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A9" s="47" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
       <c r="B9" s="48"/>
       <c r="C9" s="48"/>
       <c r="D9" s="49" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="F9" s="42"/>
       <c r="G9" s="43"/>
@@ -8875,7 +8878,7 @@
         <v>390</v>
       </c>
       <c r="D12" s="58" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F12" s="34"/>
       <c r="O12" s="37"/>
@@ -8966,7 +8969,7 @@
         <v>294</v>
       </c>
       <c r="D13" s="58" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F13" s="59"/>
       <c r="J13" s="60"/>
@@ -9060,7 +9063,7 @@
         <v>509</v>
       </c>
       <c r="D14" s="58" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F14" s="34"/>
       <c r="M14" s="60"/>
@@ -9152,7 +9155,7 @@
         <v>216</v>
       </c>
       <c r="D15" s="58" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F15" s="59"/>
       <c r="J15" s="60"/>
@@ -9247,7 +9250,7 @@
         <v>98</v>
       </c>
       <c r="D16" s="58" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F16" s="34"/>
       <c r="O16" s="37"/>
@@ -9326,7 +9329,7 @@
         <v>166</v>
       </c>
       <c r="D17" s="58" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F17" s="59"/>
       <c r="J17" s="60"/>
@@ -9417,7 +9420,7 @@
         <v>183</v>
       </c>
       <c r="D18" s="58" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F18" s="34"/>
       <c r="M18" s="60"/>
@@ -9551,7 +9554,7 @@
         <v>369</v>
       </c>
       <c r="D21" s="72" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F21" s="34"/>
       <c r="O21" s="37"/>
@@ -9642,7 +9645,7 @@
         <v>180</v>
       </c>
       <c r="D22" s="72" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F22" s="34"/>
       <c r="M22" s="60"/>
@@ -9731,7 +9734,7 @@
         <v>164</v>
       </c>
       <c r="D23" s="72" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F23" s="34"/>
       <c r="O23" s="37"/>
@@ -10181,11 +10184,11 @@
         <v>291</v>
       </c>
       <c r="D31" s="78" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="F31" s="34"/>
       <c r="K31" s="35" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="O31" s="37"/>
       <c r="P31" s="34"/>
@@ -10274,11 +10277,11 @@
         <v>122</v>
       </c>
       <c r="D32" s="78" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="F32" s="34"/>
       <c r="H32" s="35" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="O32" s="37"/>
       <c r="P32" s="34"/>
@@ -10368,11 +10371,11 @@
         <v>121</v>
       </c>
       <c r="D33" s="78" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="F33" s="34"/>
       <c r="G33" s="35" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="O33" s="37"/>
       <c r="P33" s="34"/>
@@ -10462,11 +10465,11 @@
         <v>219</v>
       </c>
       <c r="D34" s="78" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="F34" s="34"/>
       <c r="K34" s="35" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="O34" s="37"/>
       <c r="P34" s="59"/>
@@ -10553,11 +10556,11 @@
         <v>265</v>
       </c>
       <c r="D35" s="78" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="F35" s="34"/>
       <c r="L35" s="35" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="O35" s="37"/>
       <c r="P35" s="34"/>
@@ -10627,13 +10630,13 @@
         <v>57</v>
       </c>
       <c r="D36" s="78" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="F36" s="34"/>
       <c r="O36" s="37"/>
       <c r="P36" s="59"/>
       <c r="Q36" s="35" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="U36" s="60"/>
       <c r="V36" s="60"/>
@@ -10713,11 +10716,11 @@
         <v>268</v>
       </c>
       <c r="D37" s="78" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="F37" s="34"/>
       <c r="J37" s="35" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="M37" s="60"/>
       <c r="O37" s="37"/>
@@ -10808,11 +10811,11 @@
         <v>167</v>
       </c>
       <c r="D38" s="78" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="F38" s="34"/>
       <c r="K38" s="35" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="O38" s="37"/>
       <c r="P38" s="34"/>
@@ -10919,7 +10922,7 @@
         <v>76</v>
       </c>
       <c r="D41" s="83" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F41" s="34"/>
       <c r="O41" s="37"/>
@@ -10962,7 +10965,7 @@
       <c r="BD41" s="59"/>
       <c r="BE41" s="60"/>
       <c r="BF41" s="60" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="BG41" s="60"/>
       <c r="BH41" s="67"/>
@@ -11008,7 +11011,7 @@
         <v>73</v>
       </c>
       <c r="D42" s="83" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F42" s="34"/>
       <c r="O42" s="37"/>
@@ -11092,11 +11095,11 @@
         <v>16</v>
       </c>
       <c r="D43" s="83" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F43" s="34"/>
       <c r="O43" s="37" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="P43" s="34"/>
       <c r="U43" s="60"/>
@@ -11104,7 +11107,7 @@
       <c r="W43" s="60"/>
       <c r="X43" s="60"/>
       <c r="Y43" s="61" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
       <c r="Z43" s="59"/>
       <c r="AA43" s="60"/>
@@ -11183,7 +11186,7 @@
         <v>6</v>
       </c>
       <c r="D44" s="83" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F44" s="34"/>
       <c r="O44" s="37"/>
@@ -11270,11 +11273,11 @@
         <v>39</v>
       </c>
       <c r="D45" s="83" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F45" s="34"/>
       <c r="O45" s="37" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="P45" s="34"/>
       <c r="U45" s="60"/>
@@ -11405,7 +11408,7 @@
       </c>
       <c r="F48" s="34"/>
       <c r="N48" s="35" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="O48" s="37"/>
       <c r="P48" s="34"/>
@@ -11491,7 +11494,7 @@
       </c>
       <c r="F49" s="34"/>
       <c r="N49" s="35" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="O49" s="37"/>
       <c r="P49" s="34"/>
@@ -11577,7 +11580,7 @@
       </c>
       <c r="F50" s="34"/>
       <c r="O50" s="37" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="P50" s="34"/>
       <c r="Y50" s="61"/>
@@ -11662,7 +11665,7 @@
       </c>
       <c r="F51" s="34"/>
       <c r="N51" s="35" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="O51" s="37"/>
       <c r="P51" s="34"/>
@@ -11748,7 +11751,7 @@
       </c>
       <c r="F52" s="34"/>
       <c r="L52" s="35" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="O52" s="37"/>
       <c r="P52" s="34"/>
@@ -11834,7 +11837,7 @@
       </c>
       <c r="F53" s="34"/>
       <c r="N53" s="35" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="O53" s="37"/>
       <c r="P53" s="34"/>
@@ -11920,7 +11923,7 @@
       </c>
       <c r="F54" s="34"/>
       <c r="N54" s="35" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="O54" s="37"/>
       <c r="P54" s="34"/>
@@ -12044,7 +12047,7 @@
         <v>29</v>
       </c>
       <c r="D57" s="91" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="F57" s="34"/>
       <c r="O57" s="37"/>
@@ -12109,7 +12112,7 @@
         <v>183</v>
       </c>
       <c r="D58" s="91" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="F58" s="34"/>
       <c r="O58" s="37"/>
@@ -12179,7 +12182,7 @@
         <v>328</v>
       </c>
       <c r="D59" s="91" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="F59" s="34"/>
       <c r="O59" s="37"/>
@@ -12244,7 +12247,7 @@
         <v>102</v>
       </c>
       <c r="D60" s="91" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="F60" s="34"/>
       <c r="O60" s="37"/>
@@ -12341,12 +12344,12 @@
     </row>
     <row r="63" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A63" s="47" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
       <c r="B63" s="92"/>
       <c r="C63" s="5"/>
       <c r="D63" s="49" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="F63" s="34"/>
       <c r="O63" s="37"/>
@@ -12378,12 +12381,12 @@
     </row>
     <row r="64" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A64" s="47" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="B64" s="92"/>
       <c r="C64" s="5"/>
       <c r="D64" s="49" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="F64" s="34"/>
       <c r="O64" s="37"/>
@@ -12412,12 +12415,12 @@
     </row>
     <row r="65" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A65" s="47" t="s">
-        <v>350</v>
+        <v>336</v>
       </c>
       <c r="B65" s="92"/>
       <c r="C65" s="5"/>
       <c r="D65" s="49" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="F65" s="34"/>
       <c r="O65" s="37"/>
@@ -12455,12 +12458,12 @@
     </row>
     <row r="66" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A66" s="47" t="s">
-        <v>351</v>
+        <v>337</v>
       </c>
       <c r="B66" s="92"/>
       <c r="C66" s="5"/>
       <c r="D66" s="49" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="F66" s="34"/>
       <c r="O66" s="37"/>
@@ -12559,7 +12562,7 @@
       <c r="AQ68" s="60"/>
       <c r="AR68" s="60"/>
       <c r="AS68" s="61"/>
-      <c r="AT68" s="80"/>
+      <c r="AT68" s="59"/>
       <c r="AU68" s="60"/>
       <c r="AV68" s="60"/>
       <c r="AW68" s="60"/>
@@ -12574,7 +12577,7 @@
       <c r="BF68" s="60"/>
       <c r="BG68" s="60"/>
       <c r="BH68" s="60"/>
-      <c r="BI68" s="60"/>
+      <c r="BI68" s="67"/>
       <c r="BJ68" s="60"/>
       <c r="BK68" s="60"/>
       <c r="BL68" s="60"/>
@@ -12993,7 +12996,7 @@
       <c r="BI74" s="60"/>
       <c r="BJ74" s="60"/>
       <c r="BK74" s="60" t="s">
-        <v>352</v>
+        <v>338</v>
       </c>
       <c r="BL74" s="60"/>
       <c r="BM74" s="62"/>
@@ -13066,12 +13069,12 @@
     </row>
     <row r="77" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A77" s="47" t="s">
-        <v>353</v>
+        <v>339</v>
       </c>
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
       <c r="D77" s="49" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="F77" s="34"/>
       <c r="O77" s="37"/>
@@ -13100,12 +13103,12 @@
     </row>
     <row r="78" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A78" s="47" t="s">
-        <v>354</v>
+        <v>340</v>
       </c>
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
       <c r="D78" s="49" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="F78" s="34"/>
       <c r="O78" s="37"/>
@@ -13172,12 +13175,12 @@
     </row>
     <row r="79" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A79" s="47" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
       <c r="D79" s="49" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="F79" s="34"/>
       <c r="O79" s="37"/>
@@ -13253,7 +13256,7 @@
         <v>26</v>
       </c>
       <c r="D82" s="109" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="F82" s="34"/>
       <c r="O82" s="37"/>
@@ -13312,7 +13315,7 @@
         <v>11</v>
       </c>
       <c r="D83" s="109" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="F83" s="34"/>
       <c r="O83" s="37"/>
@@ -13324,7 +13327,7 @@
       <c r="AS83" s="37"/>
       <c r="AT83" s="34"/>
       <c r="BC83" s="37" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="BD83" s="34"/>
       <c r="BF83" s="60"/>
@@ -13372,7 +13375,7 @@
         <v>12</v>
       </c>
       <c r="D84" s="109" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="F84" s="34"/>
       <c r="O84" s="37"/>
@@ -13383,7 +13386,7 @@
       <c r="AJ84" s="34"/>
       <c r="AS84" s="37"/>
       <c r="AT84" s="34" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="BC84" s="61"/>
       <c r="BD84" s="59"/>
@@ -13433,7 +13436,7 @@
         <v>23</v>
       </c>
       <c r="D85" s="109" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="F85" s="34"/>
       <c r="O85" s="37"/>
@@ -13441,7 +13444,7 @@
       <c r="Y85" s="37"/>
       <c r="Z85" s="34"/>
       <c r="AC85" s="35" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="AI85" s="37"/>
       <c r="AJ85" s="34"/>
@@ -13495,14 +13498,14 @@
         <v>169</v>
       </c>
       <c r="D86" s="109" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="F86" s="34"/>
       <c r="O86" s="37"/>
       <c r="P86" s="34"/>
       <c r="Y86" s="37"/>
       <c r="Z86" s="34" t="s">
-        <v>356</v>
+        <v>342</v>
       </c>
       <c r="AI86" s="37"/>
       <c r="AJ86" s="34"/>
@@ -13556,7 +13559,7 @@
         <v>6</v>
       </c>
       <c r="D87" s="109" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="F87" s="34"/>
       <c r="O87" s="37"/>
@@ -13568,7 +13571,7 @@
       <c r="AS87" s="37"/>
       <c r="AT87" s="34"/>
       <c r="AX87" s="35" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="BC87" s="61"/>
       <c r="BD87" s="59"/>
@@ -13618,7 +13621,7 @@
         <v>18</v>
       </c>
       <c r="D88" s="109" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="F88" s="34"/>
       <c r="O88" s="37"/>
@@ -13628,7 +13631,7 @@
       <c r="AI88" s="37"/>
       <c r="AJ88" s="34"/>
       <c r="AM88" s="35" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="AS88" s="37"/>
       <c r="AT88" s="34"/>
@@ -13721,7 +13724,7 @@
         <v>54</v>
       </c>
       <c r="D91" s="112" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="F91" s="34"/>
       <c r="O91" s="37"/>
@@ -13744,7 +13747,7 @@
     </row>
     <row r="92" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A92" s="110" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B92" s="111" t="s">
         <v>54</v>
@@ -13753,7 +13756,7 @@
         <v>54</v>
       </c>
       <c r="D92" s="112" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="F92" s="34"/>
       <c r="O92" s="37"/>

</xml_diff>